<commit_message>
fixed the palochkas in Sanzhi
</commit_message>
<xml_diff>
--- a/lists/sanzhi.xlsx
+++ b/lists/sanzhi.xlsx
@@ -11,12 +11,12 @@
     <sheet name="lexcauc" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$AD$2139</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$K$2139</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">lexcauc!$I$1:$K$2724</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters_1" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters_2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$K$2139</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$AD$2139</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -222,7 +222,7 @@
     <t xml:space="preserve">EARTH</t>
   </si>
   <si>
-    <t xml:space="preserve">г1янччи</t>
+    <t xml:space="preserve">гӀянччи</t>
   </si>
   <si>
     <t xml:space="preserve">ʡaˁnčːi</t>
@@ -354,7 +354,7 @@
     <t xml:space="preserve">CLIFF</t>
   </si>
   <si>
-    <t xml:space="preserve">хъич1а </t>
+    <t xml:space="preserve">хъичӀа </t>
   </si>
   <si>
     <t xml:space="preserve">qičʼa</t>
@@ -363,7 +363,7 @@
     <t xml:space="preserve">q͡χʰit͡ʃʼa</t>
   </si>
   <si>
-    <t xml:space="preserve">хъич1ме</t>
+    <t xml:space="preserve">хъичӀме</t>
   </si>
   <si>
     <t xml:space="preserve">qičʼ-me</t>
@@ -486,7 +486,7 @@
     <t xml:space="preserve">RIVER</t>
   </si>
   <si>
-    <t xml:space="preserve">эрк1в</t>
+    <t xml:space="preserve">эркӀв</t>
   </si>
   <si>
     <t xml:space="preserve">erkʼʷ</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">ʔerkʼʷ</t>
   </si>
   <si>
-    <t xml:space="preserve">эрк1вме</t>
+    <t xml:space="preserve">эркӀвме</t>
   </si>
   <si>
     <t xml:space="preserve">erkʼʷme</t>
@@ -561,7 +561,7 @@
     <t xml:space="preserve">FOREST</t>
   </si>
   <si>
-    <t xml:space="preserve">вац1а</t>
+    <t xml:space="preserve">вацӀа</t>
   </si>
   <si>
     <t xml:space="preserve">wacʼa</t>
@@ -570,7 +570,7 @@
     <t xml:space="preserve">wat͡sʼa</t>
   </si>
   <si>
-    <t xml:space="preserve">вац1урбе</t>
+    <t xml:space="preserve">вацӀурбе</t>
   </si>
   <si>
     <t xml:space="preserve">wacʼur-be</t>
@@ -699,7 +699,7 @@
     <t xml:space="preserve">LIGHTNING</t>
   </si>
   <si>
-    <t xml:space="preserve">лямц1</t>
+    <t xml:space="preserve">лямцӀ</t>
   </si>
   <si>
     <t xml:space="preserve">laˁmcʼ</t>
@@ -708,7 +708,7 @@
     <t xml:space="preserve">laˁmt͡sʼ</t>
   </si>
   <si>
-    <t xml:space="preserve">лямц1не</t>
+    <t xml:space="preserve">лямцӀне</t>
   </si>
   <si>
     <t xml:space="preserve">laˁmcʼ-ne</t>
@@ -765,7 +765,7 @@
     <t xml:space="preserve">SHADOW</t>
   </si>
   <si>
-    <t xml:space="preserve">бях1тти</t>
+    <t xml:space="preserve">бяхӀтти</t>
   </si>
   <si>
     <t xml:space="preserve">baˁħtːi</t>
@@ -798,7 +798,7 @@
     <t xml:space="preserve">WIND</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ан</t>
+    <t xml:space="preserve">чӀан</t>
   </si>
   <si>
     <t xml:space="preserve">čʼan</t>
@@ -861,7 +861,7 @@
     <t xml:space="preserve">SNOW</t>
   </si>
   <si>
-    <t xml:space="preserve">ду1х1и</t>
+    <t xml:space="preserve">дуӀхӀи</t>
   </si>
   <si>
     <t xml:space="preserve">duˁħi</t>
@@ -963,13 +963,13 @@
     <t xml:space="preserve">MELT (INTR)</t>
   </si>
   <si>
-    <t xml:space="preserve">бац1ий</t>
+    <t xml:space="preserve">бацӀий</t>
   </si>
   <si>
     <t xml:space="preserve">bat͡sʼij</t>
   </si>
   <si>
-    <t xml:space="preserve">биц1ий</t>
+    <t xml:space="preserve">бицӀий</t>
   </si>
   <si>
     <t xml:space="preserve">bit͡sʼij</t>
@@ -981,13 +981,13 @@
     <t xml:space="preserve">MELT (TR)</t>
   </si>
   <si>
-    <t xml:space="preserve">бац1ахъий</t>
+    <t xml:space="preserve">бацӀахъий</t>
   </si>
   <si>
     <t xml:space="preserve">bat͡sʼaq͡χʰij</t>
   </si>
   <si>
-    <t xml:space="preserve">биц1ахъий</t>
+    <t xml:space="preserve">бицӀахъий</t>
   </si>
   <si>
     <t xml:space="preserve">bit͡sʼaq͡χʰij</t>
@@ -999,7 +999,7 @@
     <t xml:space="preserve">FIRE</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1а</t>
+    <t xml:space="preserve">цӀа</t>
   </si>
   <si>
     <t xml:space="preserve">t͡sʼa</t>
@@ -1128,13 +1128,13 @@
     <t xml:space="preserve">BECOME COLD</t>
   </si>
   <si>
-    <t xml:space="preserve">бярг1ий</t>
+    <t xml:space="preserve">бяргӀий</t>
   </si>
   <si>
     <t xml:space="preserve">baˁrʡij</t>
   </si>
   <si>
-    <t xml:space="preserve">бирг1ий</t>
+    <t xml:space="preserve">биргӀий</t>
   </si>
   <si>
     <t xml:space="preserve">birʡij</t>
@@ -1248,13 +1248,13 @@
     <t xml:space="preserve">BOY</t>
   </si>
   <si>
-    <t xml:space="preserve">дурх1у1</t>
+    <t xml:space="preserve">дурхӀуӀ</t>
   </si>
   <si>
     <t xml:space="preserve">durħuˁ</t>
   </si>
   <si>
-    <t xml:space="preserve">дурх1не</t>
+    <t xml:space="preserve">дурхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">durħne</t>
@@ -1284,10 +1284,10 @@
     <t xml:space="preserve">INFANT</t>
   </si>
   <si>
-    <t xml:space="preserve">ник1а дурх1у1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ник1а дурх1не</t>
+    <t xml:space="preserve">никӀа дурхӀуӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">никӀа дурхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">МУЖ</t>
@@ -1314,10 +1314,10 @@
     <t xml:space="preserve">BRIDE</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1икури</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ц1икурме</t>
+    <t xml:space="preserve">цӀикури</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цӀикурме</t>
   </si>
   <si>
     <t xml:space="preserve">ЖЕНИХ</t>
@@ -1350,7 +1350,7 @@
     <t xml:space="preserve">MARRY (AS WOMAN)</t>
   </si>
   <si>
-    <t xml:space="preserve">хьади ру1кьий</t>
+    <t xml:space="preserve">хьади руӀкьий</t>
   </si>
   <si>
     <t xml:space="preserve">хьади раший</t>
@@ -1446,7 +1446,7 @@
     <t xml:space="preserve">TWINS</t>
   </si>
   <si>
-    <t xml:space="preserve">к1видаркьи</t>
+    <t xml:space="preserve">кӀвидаркьи</t>
   </si>
   <si>
     <t xml:space="preserve">ДЕДУШКА (ОТЕЦ ОТЦА)</t>
@@ -1509,10 +1509,10 @@
     <t xml:space="preserve">GRANDSON (SON OF SON)</t>
   </si>
   <si>
-    <t xml:space="preserve">дурх1улла дурх1у</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дурх1улла дурх1не</t>
+    <t xml:space="preserve">дурхӀулла дурхӀу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дурхӀулла дурхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ВНУК (СЫН ДОЧЕРИ)</t>
@@ -1521,10 +1521,10 @@
     <t xml:space="preserve">GRANDSON (SON OF DAUGHTER)</t>
   </si>
   <si>
-    <t xml:space="preserve">рурссила дурх1у</t>
-  </si>
-  <si>
-    <t xml:space="preserve">рурссила дурх1не</t>
+    <t xml:space="preserve">рурссила дурхӀу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">рурссила дурхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ВНУЧКА (ДОЧЬ СЫНА)</t>
@@ -1533,10 +1533,10 @@
     <t xml:space="preserve">GRANDDAUGHTER (DAUGHTER OF SON)</t>
   </si>
   <si>
-    <t xml:space="preserve">дурх1улла рурсси</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дурх1улла рурсбе</t>
+    <t xml:space="preserve">дурхӀулла рурсси</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дурхӀулла рурсбе</t>
   </si>
   <si>
     <t xml:space="preserve">ВНУЧКА (ДОЧЬ ДОЧЕРИ)</t>
@@ -1695,10 +1695,10 @@
     <t xml:space="preserve">DAUGHTER-IN-LAW (OF A MAN)</t>
   </si>
   <si>
-    <t xml:space="preserve">дурх1ёла хьхьунул</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дурх1ёла хьхьунре</t>
+    <t xml:space="preserve">дурхӀёла хьхьунул</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дурхӀёла хьхьунре</t>
   </si>
   <si>
     <t xml:space="preserve">НЕВЕСТКА</t>
@@ -1713,7 +1713,7 @@
     <t xml:space="preserve">STEPFATHER</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яххёл атта</t>
+    <t xml:space="preserve">гӀяххёл атта</t>
   </si>
   <si>
     <r>
@@ -1765,7 +1765,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">г1яххёл атне</t>
+    <t xml:space="preserve">гӀяххёл атне</t>
   </si>
   <si>
     <t xml:space="preserve">угай атта</t>
@@ -1780,10 +1780,10 @@
     <t xml:space="preserve">STEPMOTHER</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яххёл аба</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1яххёл абне</t>
+    <t xml:space="preserve">гӀяххёл аба</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяххёл абне</t>
   </si>
   <si>
     <t xml:space="preserve">угай аба</t>
@@ -1798,16 +1798,16 @@
     <t xml:space="preserve">STEPSON</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яххёл дурх1ё</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1яххёл дурх1не</t>
-  </si>
-  <si>
-    <t xml:space="preserve">угай дурх1ё</t>
-  </si>
-  <si>
-    <t xml:space="preserve">угай дурх1не</t>
+    <t xml:space="preserve">гӀяххёл дурхӀё</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяххёл дурхӀне</t>
+  </si>
+  <si>
+    <t xml:space="preserve">угай дурхӀё</t>
+  </si>
+  <si>
+    <t xml:space="preserve">угай дурхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ПАДЧЕРИЦА</t>
@@ -1816,10 +1816,10 @@
     <t xml:space="preserve">STEPDAUGHTER</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яххёл рурсси</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1яххёл рурсбе</t>
+    <t xml:space="preserve">гӀяххёл рурсси</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяххёл рурсбе</t>
   </si>
   <si>
     <t xml:space="preserve">угай рурсси</t>
@@ -2059,7 +2059,7 @@
     <t xml:space="preserve">LIVESTOCK</t>
   </si>
   <si>
-    <t xml:space="preserve">х1яйванте</t>
+    <t xml:space="preserve">хӀяйванте</t>
   </si>
   <si>
     <t xml:space="preserve">ПАСТБИЩЕ (ЛЕТНЕЕ)</t>
@@ -2068,13 +2068,13 @@
     <t xml:space="preserve">PASTURE (SUMMER)</t>
   </si>
   <si>
-    <t xml:space="preserve">кьят1</t>
+    <t xml:space="preserve">кьятӀ</t>
   </si>
   <si>
     <t xml:space="preserve">this is not the summer pasture; HM does not really know this word because the word 'pasturing' is usually used</t>
   </si>
   <si>
-    <t xml:space="preserve">кьят1не</t>
+    <t xml:space="preserve">кьятӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ПАСТУХ (КОРОВ)</t>
@@ -2167,10 +2167,10 @@
     <t xml:space="preserve">SHEAF</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ябкьигар</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ябкьигарме</t>
+    <t xml:space="preserve">гӀябкьигар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀябкьигарме</t>
   </si>
   <si>
     <t xml:space="preserve">СТОГ</t>
@@ -2200,7 +2200,7 @@
     <t xml:space="preserve">кьвял</t>
   </si>
   <si>
-    <t xml:space="preserve">кьу1ле</t>
+    <t xml:space="preserve">кьуӀле</t>
   </si>
   <si>
     <t xml:space="preserve">БЫК</t>
@@ -2233,10 +2233,10 @@
     <t xml:space="preserve">HEIFER</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ахъа</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1ахъне</t>
+    <t xml:space="preserve">кӀахъа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀахъне</t>
   </si>
   <si>
     <t xml:space="preserve">БЫЧОК</t>
@@ -2245,10 +2245,10 @@
     <t xml:space="preserve">BULL-CALF</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ашша</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1ушме</t>
+    <t xml:space="preserve">кӀашша</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀушме</t>
   </si>
   <si>
     <t xml:space="preserve">ТЕЛЁНОК</t>
@@ -2428,10 +2428,10 @@
     <t xml:space="preserve">FOAL</t>
   </si>
   <si>
-    <t xml:space="preserve">тяг1яй</t>
-  </si>
-  <si>
-    <t xml:space="preserve">тяг1яйте</t>
+    <t xml:space="preserve">тягӀяй</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тягӀяйте</t>
   </si>
   <si>
     <t xml:space="preserve">ОСЕЛ</t>
@@ -2488,10 +2488,10 @@
     <t xml:space="preserve">HEN</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ярг1я</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1у1рг1е</t>
+    <t xml:space="preserve">гӀяргӀя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀуӀргӀе</t>
   </si>
   <si>
     <t xml:space="preserve">ЦЫПЛЁНОК</t>
@@ -2500,10 +2500,10 @@
     <t xml:space="preserve">CHICK</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1игва</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ч1игвне</t>
+    <t xml:space="preserve">чӀигва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чӀигвне</t>
   </si>
   <si>
     <t xml:space="preserve">ГУСЬ</t>
@@ -2524,7 +2524,7 @@
     <t xml:space="preserve">DUCK</t>
   </si>
   <si>
-    <t xml:space="preserve">бят1бят1</t>
+    <t xml:space="preserve">бятӀбятӀ</t>
   </si>
   <si>
     <t xml:space="preserve">домашняя утка</t>
@@ -2533,7 +2533,7 @@
     <t xml:space="preserve">domestic duck</t>
   </si>
   <si>
-    <t xml:space="preserve">бят1бят1е</t>
+    <t xml:space="preserve">бятӀбятӀе</t>
   </si>
   <si>
     <t xml:space="preserve">урдек</t>
@@ -2590,10 +2590,10 @@
     <t xml:space="preserve">EAGLE</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ака</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ч1акне</t>
+    <t xml:space="preserve">чӀака</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чӀакне</t>
   </si>
   <si>
     <t xml:space="preserve">ЯСТРЕБ</t>
@@ -2632,10 +2632,10 @@
     <t xml:space="preserve">BAT</t>
   </si>
   <si>
-    <t xml:space="preserve">х1якапутти</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1якапутне</t>
+    <t xml:space="preserve">хӀякапутти</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀякапутне</t>
   </si>
   <si>
     <t xml:space="preserve">ВОРОНА</t>
@@ -2698,10 +2698,10 @@
     <t xml:space="preserve">OWL</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ума</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1умре</t>
+    <t xml:space="preserve">тӀума</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀумре</t>
   </si>
   <si>
     <t xml:space="preserve">ФИЛИН</t>
@@ -2752,13 +2752,13 @@
     <t xml:space="preserve">жатне</t>
   </si>
   <si>
-    <t xml:space="preserve">х1яжила жатта</t>
+    <t xml:space="preserve">хӀяжила жатта</t>
   </si>
   <si>
     <t xml:space="preserve">Without the first word the meaning is identical, i.e. the first word is optional.</t>
   </si>
   <si>
-    <t xml:space="preserve">х1яжила жатне</t>
+    <t xml:space="preserve">хӀяжила жатне</t>
   </si>
   <si>
     <t xml:space="preserve">СОБАКА</t>
@@ -2797,10 +2797,10 @@
     <t xml:space="preserve">PUPPY OF DOG</t>
   </si>
   <si>
-    <t xml:space="preserve">кац1и</t>
-  </si>
-  <si>
-    <t xml:space="preserve">кац1не</t>
+    <t xml:space="preserve">кацӀи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кацӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ЗАЯЦ</t>
@@ -2809,10 +2809,10 @@
     <t xml:space="preserve">HARE</t>
   </si>
   <si>
-    <t xml:space="preserve">гъу1ра</t>
-  </si>
-  <si>
-    <t xml:space="preserve">гъу1рне</t>
+    <t xml:space="preserve">гъуӀра</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гъуӀрне</t>
   </si>
   <si>
     <t xml:space="preserve">КОШКА</t>
@@ -2857,10 +2857,10 @@
     <t xml:space="preserve">BADGER</t>
   </si>
   <si>
-    <t xml:space="preserve">т1уж</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1ужме</t>
+    <t xml:space="preserve">тӀуж</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀужме</t>
   </si>
   <si>
     <t xml:space="preserve">КУНИЦА</t>
@@ -2869,10 +2869,10 @@
     <t xml:space="preserve">MARTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">хярц1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хярц1ме</t>
+    <t xml:space="preserve">хярцӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хярцӀме</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛКА</t>
@@ -2881,10 +2881,10 @@
     <t xml:space="preserve">SQUIRREL</t>
   </si>
   <si>
-    <t xml:space="preserve">йярмала ч1ими</t>
-  </si>
-  <si>
-    <t xml:space="preserve">йярмала ч1имре</t>
+    <t xml:space="preserve">йярмала чӀими</t>
+  </si>
+  <si>
+    <t xml:space="preserve">йярмала чӀимре</t>
   </si>
   <si>
     <t xml:space="preserve">ЁЖ</t>
@@ -2923,10 +2923,10 @@
     <t xml:space="preserve">WOLF</t>
   </si>
   <si>
-    <t xml:space="preserve">бец1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">буц1е</t>
+    <t xml:space="preserve">бецӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">буцӀе</t>
   </si>
   <si>
     <t xml:space="preserve">МЕДВЕДЬ</t>
@@ -2983,10 +2983,10 @@
     <t xml:space="preserve">ROE</t>
   </si>
   <si>
-    <t xml:space="preserve">хьвент1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хьвент1не</t>
+    <t xml:space="preserve">хьвентӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хьвентӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ВЕРБЛЮД</t>
@@ -3037,10 +3037,10 @@
     <t xml:space="preserve">FLEA</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1ика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ц1икне</t>
+    <t xml:space="preserve">цӀика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цӀикне</t>
   </si>
   <si>
     <t xml:space="preserve">ПИЯВКА</t>
@@ -3049,10 +3049,10 @@
     <t xml:space="preserve">LEECH</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1иц1бухъ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ц1иц1букъе</t>
+    <t xml:space="preserve">цӀицӀбухъ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цӀицӀбукъе</t>
   </si>
   <si>
     <t xml:space="preserve">МУРАВЕЙ</t>
@@ -3103,10 +3103,10 @@
     <t xml:space="preserve">MITE</t>
   </si>
   <si>
-    <t xml:space="preserve">сассак1ар</t>
-  </si>
-  <si>
-    <t xml:space="preserve">сассук1ре</t>
+    <t xml:space="preserve">сассакӀар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сассукӀре</t>
   </si>
   <si>
     <t xml:space="preserve">КЛОП</t>
@@ -3163,10 +3163,10 @@
     <t xml:space="preserve">BEESWAX</t>
   </si>
   <si>
-    <t xml:space="preserve">мурч1ал</t>
-  </si>
-  <si>
-    <t xml:space="preserve">мурч1ле</t>
+    <t xml:space="preserve">мурчӀал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">мурчӀле</t>
   </si>
   <si>
     <t xml:space="preserve">УЛЕЙ</t>
@@ -3175,13 +3175,13 @@
     <t xml:space="preserve">BEEHIVE</t>
   </si>
   <si>
-    <t xml:space="preserve">мирхъила т1уннехъ</t>
+    <t xml:space="preserve">мирхъила тӀуннехъ</t>
   </si>
   <si>
     <t xml:space="preserve">this word needs to be rechecked</t>
   </si>
   <si>
-    <t xml:space="preserve">мирхъила т1уннухъ</t>
+    <t xml:space="preserve">мирхъила тӀуннухъ</t>
   </si>
   <si>
     <t xml:space="preserve">ОСА</t>
@@ -3202,13 +3202,13 @@
     <t xml:space="preserve">FLY</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ат1ар</t>
+    <t xml:space="preserve">тӀатӀар</t>
   </si>
   <si>
     <t xml:space="preserve">tʼatʼar</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ат1ре</t>
+    <t xml:space="preserve">тӀатӀре</t>
   </si>
   <si>
     <t xml:space="preserve">tʼatʼre</t>
@@ -3250,13 +3250,13 @@
     <t xml:space="preserve">SNAKE</t>
   </si>
   <si>
-    <t xml:space="preserve">мялг1юн</t>
+    <t xml:space="preserve">мялгӀюн</t>
   </si>
   <si>
     <t xml:space="preserve">maˁlʡuˁn</t>
   </si>
   <si>
-    <t xml:space="preserve">мялг1юнте</t>
+    <t xml:space="preserve">мялгӀюнте</t>
   </si>
   <si>
     <t xml:space="preserve">maˁlʡuˁnte</t>
@@ -3268,10 +3268,10 @@
     <t xml:space="preserve">FIREFLY</t>
   </si>
   <si>
-    <t xml:space="preserve">дуччи лямц1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дуччи лямц1бе</t>
+    <t xml:space="preserve">дуччи лямцӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дуччи лямцӀбе</t>
   </si>
   <si>
     <t xml:space="preserve">шшала мирихъв</t>
@@ -3286,10 +3286,10 @@
     <t xml:space="preserve">BUTTERFLY</t>
   </si>
   <si>
-    <t xml:space="preserve">алх1ян</t>
-  </si>
-  <si>
-    <t xml:space="preserve">алх1янте</t>
+    <t xml:space="preserve">алхӀян</t>
+  </si>
+  <si>
+    <t xml:space="preserve">алхӀянте</t>
   </si>
   <si>
     <t xml:space="preserve">КУЗНЕЧИК</t>
@@ -3316,10 +3316,10 @@
     <t xml:space="preserve">FROG</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ят1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ят1не</t>
+    <t xml:space="preserve">гӀятӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀятӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ЯЩЕРИЦА</t>
@@ -3337,10 +3337,10 @@
     <t xml:space="preserve">гьелкъне</t>
   </si>
   <si>
-    <t xml:space="preserve">шшят1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">шшят1не</t>
+    <t xml:space="preserve">шшятӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">шшятӀне</t>
   </si>
   <si>
     <t xml:space="preserve">МЫЧАТЬ</t>
@@ -3349,7 +3349,7 @@
     <t xml:space="preserve">MOO</t>
   </si>
   <si>
-    <t xml:space="preserve">му бик1вий</t>
+    <t xml:space="preserve">му бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">БЛЕЯТЬ (ОВЦА)</t>
@@ -3358,7 +3358,7 @@
     <t xml:space="preserve">BLEAT (SHEEP)</t>
   </si>
   <si>
-    <t xml:space="preserve">мя бик1вий</t>
+    <t xml:space="preserve">мя бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">БЛЕЯТЬ (КОЗА)</t>
@@ -3367,7 +3367,7 @@
     <t xml:space="preserve">BLEAT (GOAT)</t>
   </si>
   <si>
-    <t xml:space="preserve">бя бик1вий</t>
+    <t xml:space="preserve">бя бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">РЖАТЬ</t>
@@ -3376,7 +3376,7 @@
     <t xml:space="preserve">NEIGH</t>
   </si>
   <si>
-    <t xml:space="preserve">и бик1вий</t>
+    <t xml:space="preserve">и бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">КРИЧАТЬ (ОСЁЛ)</t>
@@ -3385,7 +3385,7 @@
     <t xml:space="preserve">HEE-HAW</t>
   </si>
   <si>
-    <t xml:space="preserve">х1у1г1 бик1вий</t>
+    <t xml:space="preserve">хӀуӀгӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">МЯУКАТЬ</t>
@@ -3394,7 +3394,7 @@
     <t xml:space="preserve">MEAOW</t>
   </si>
   <si>
-    <t xml:space="preserve">мяв бик1вий</t>
+    <t xml:space="preserve">мяв бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ЛАЯТЬ</t>
@@ -3403,7 +3403,7 @@
     <t xml:space="preserve">BARK (V.)</t>
   </si>
   <si>
-    <t xml:space="preserve">гъям бик1вий</t>
+    <t xml:space="preserve">гъям бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">РЫЧАТЬ</t>
@@ -3412,7 +3412,7 @@
     <t xml:space="preserve">ROAR</t>
   </si>
   <si>
-    <t xml:space="preserve">гъугъ бик1вий</t>
+    <t xml:space="preserve">гъугъ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ВЫТЬ</t>
@@ -3421,13 +3421,13 @@
     <t xml:space="preserve">HOWL</t>
   </si>
   <si>
-    <t xml:space="preserve">гьав бик1вий</t>
+    <t xml:space="preserve">гьав бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">КУКАРЕКАТЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ёг1ёг1ё бик1вий</t>
+    <t xml:space="preserve">гӀёгӀёгӀё бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ЖУЖЖАТЬ</t>
@@ -3436,7 +3436,7 @@
     <t xml:space="preserve">BUZZ</t>
   </si>
   <si>
-    <t xml:space="preserve">зиз бик1вий</t>
+    <t xml:space="preserve">зиз бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ШИПЕТЬ</t>
@@ -3445,7 +3445,7 @@
     <t xml:space="preserve">HISS</t>
   </si>
   <si>
-    <t xml:space="preserve">шш бик1вий</t>
+    <t xml:space="preserve">шш бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ТЕЛО</t>
@@ -3583,10 +3583,10 @@
     <t xml:space="preserve">BEARD</t>
   </si>
   <si>
-    <t xml:space="preserve">муц1ур</t>
-  </si>
-  <si>
-    <t xml:space="preserve">муц1урбе</t>
+    <t xml:space="preserve">муцӀур</t>
+  </si>
+  <si>
+    <t xml:space="preserve">муцӀурбе</t>
   </si>
   <si>
     <t xml:space="preserve">УСЫ</t>
@@ -3631,7 +3631,7 @@
     <t xml:space="preserve">DANDRUFF</t>
   </si>
   <si>
-    <t xml:space="preserve">бек1ла кам</t>
+    <t xml:space="preserve">бекӀла кам</t>
   </si>
   <si>
     <t xml:space="preserve">КРОВЬ</t>
@@ -3676,10 +3676,10 @@
     <t xml:space="preserve">JOINT</t>
   </si>
   <si>
-    <t xml:space="preserve">бирк1ун</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дирк1унте</t>
+    <t xml:space="preserve">биркӀун</t>
+  </si>
+  <si>
+    <t xml:space="preserve">диркӀунте</t>
   </si>
   <si>
     <t xml:space="preserve">ХРЯЩ</t>
@@ -3688,10 +3688,10 @@
     <t xml:space="preserve">CARTILAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">хъамссик1в</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хъамссик1ве</t>
+    <t xml:space="preserve">хъамссикӀв</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хъамссикӀве</t>
   </si>
   <si>
     <t xml:space="preserve">ЖЕЛЧЬ</t>
@@ -3727,7 +3727,7 @@
     <t xml:space="preserve">LIQUID STOOL</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1их</t>
+    <t xml:space="preserve">цӀих</t>
   </si>
   <si>
     <t xml:space="preserve">ПОМЁТ КОРОВЫ</t>
@@ -3736,7 +3736,7 @@
     <t xml:space="preserve">DUNG (OF COW)</t>
   </si>
   <si>
-    <t xml:space="preserve">п1ялц1а</t>
+    <t xml:space="preserve">пӀялцӀа</t>
   </si>
   <si>
     <t xml:space="preserve">This is the word for the liquid dung (manure).</t>
@@ -3796,13 +3796,13 @@
     <t xml:space="preserve">TAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ими</t>
+    <t xml:space="preserve">чӀими</t>
   </si>
   <si>
     <t xml:space="preserve">čʼimi</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1имре</t>
+    <t xml:space="preserve">чӀимре</t>
   </si>
   <si>
     <t xml:space="preserve">čʼimre</t>
@@ -3853,13 +3853,13 @@
     <t xml:space="preserve">HEAD</t>
   </si>
   <si>
-    <t xml:space="preserve">бек1</t>
+    <t xml:space="preserve">бекӀ</t>
   </si>
   <si>
     <t xml:space="preserve">bekʼ</t>
   </si>
   <si>
-    <t xml:space="preserve">бук1е</t>
+    <t xml:space="preserve">букӀе</t>
   </si>
   <si>
     <t xml:space="preserve">bukʼe</t>
@@ -3883,10 +3883,10 @@
     <t xml:space="preserve">SKULL</t>
   </si>
   <si>
-    <t xml:space="preserve">бек1ла вакъа</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бек1ла вахъне</t>
+    <t xml:space="preserve">бекӀла вакъа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бекӀла вахъне</t>
   </si>
   <si>
     <t xml:space="preserve">МОЗГ ГОЛОВНОЙ</t>
@@ -3970,10 +3970,10 @@
     <t xml:space="preserve">FACE</t>
   </si>
   <si>
-    <t xml:space="preserve">дяг1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дёг1ре</t>
+    <t xml:space="preserve">дягӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дёгӀре</t>
   </si>
   <si>
     <t xml:space="preserve">ЛОБ</t>
@@ -4063,7 +4063,7 @@
     <t xml:space="preserve">laˁp</t>
   </si>
   <si>
-    <t xml:space="preserve">лу1ппе</t>
+    <t xml:space="preserve">луӀппе</t>
   </si>
   <si>
     <t xml:space="preserve">luˁpːe</t>
@@ -4090,7 +4090,7 @@
     <t xml:space="preserve">qːuˁnq</t>
   </si>
   <si>
-    <t xml:space="preserve">къу1нхъуппе</t>
+    <t xml:space="preserve">къуӀнхъуппе</t>
   </si>
   <si>
     <t xml:space="preserve">qːuˁnqbe</t>
@@ -4105,7 +4105,7 @@
     <t xml:space="preserve">SNIVEL</t>
   </si>
   <si>
-    <t xml:space="preserve">г1юнзе</t>
+    <t xml:space="preserve">гӀюнзе</t>
   </si>
   <si>
     <t xml:space="preserve">what is ‹ю›? is it the same as ‹ё›?</t>
@@ -4156,10 +4156,10 @@
     <t xml:space="preserve">LIP</t>
   </si>
   <si>
-    <t xml:space="preserve">к1вент1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1унт1бе</t>
+    <t xml:space="preserve">кӀвентӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀунтӀбе</t>
   </si>
   <si>
     <t xml:space="preserve">ЯЗЫК (ОРГАН)</t>
@@ -4249,10 +4249,10 @@
     <t xml:space="preserve">ADAM’S APPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">сусла кьу1та</t>
-  </si>
-  <si>
-    <t xml:space="preserve">сусла кьу1тне</t>
+    <t xml:space="preserve">сусла кьуӀта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сусла кьуӀтне</t>
   </si>
   <si>
     <t xml:space="preserve">ПОДБОРОДОК</t>
@@ -4261,10 +4261,10 @@
     <t xml:space="preserve">CHIN</t>
   </si>
   <si>
-    <t xml:space="preserve">муц1урра гула</t>
-  </si>
-  <si>
-    <t xml:space="preserve">муц1урра гулме</t>
+    <t xml:space="preserve">муцӀурра гула</t>
+  </si>
+  <si>
+    <t xml:space="preserve">муцӀурра гулме</t>
   </si>
   <si>
     <t xml:space="preserve">ЗАТЫЛОК</t>
@@ -4273,10 +4273,10 @@
     <t xml:space="preserve">BACK OF HEAD</t>
   </si>
   <si>
-    <t xml:space="preserve">бек1ла гьила</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бек1ла гьиламе</t>
+    <t xml:space="preserve">бекӀла гьила</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бекӀла гьиламе</t>
   </si>
   <si>
     <t xml:space="preserve">ГОРЛО</t>
@@ -4309,10 +4309,10 @@
     <t xml:space="preserve">SHOULDER</t>
   </si>
   <si>
-    <t xml:space="preserve">хъурч1ул</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хъурч1ле</t>
+    <t xml:space="preserve">хъурчӀул</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хъурчӀле</t>
   </si>
   <si>
     <t xml:space="preserve">РУКА</t>
@@ -4369,10 +4369,10 @@
     <t xml:space="preserve">PAW</t>
   </si>
   <si>
-    <t xml:space="preserve">квач1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">квач1ме</t>
+    <t xml:space="preserve">квачӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">квачӀме</t>
   </si>
   <si>
     <t xml:space="preserve">КУЛАК</t>
@@ -4429,10 +4429,10 @@
     <t xml:space="preserve">FINGER</t>
   </si>
   <si>
-    <t xml:space="preserve">т1уп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1уппе</t>
+    <t xml:space="preserve">тӀуп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀуппе</t>
   </si>
   <si>
     <t xml:space="preserve">НОГОТЬ</t>
@@ -4465,13 +4465,13 @@
     <t xml:space="preserve">LEG</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ю</t>
+    <t xml:space="preserve">тӀю</t>
   </si>
   <si>
     <t xml:space="preserve">tʼuˁ</t>
   </si>
   <si>
-    <t xml:space="preserve">т1у1ме</t>
+    <t xml:space="preserve">тӀуӀме</t>
   </si>
   <si>
     <t xml:space="preserve">tʼuˁme</t>
@@ -4507,10 +4507,10 @@
     <t xml:space="preserve">SHIN</t>
   </si>
   <si>
-    <t xml:space="preserve">т1у1ла ликка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1у1ла ликне</t>
+    <t xml:space="preserve">тӀуӀла ликка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀуӀла ликне</t>
   </si>
   <si>
     <t xml:space="preserve">КОЛЕНО</t>
@@ -4549,13 +4549,13 @@
     <t xml:space="preserve">FOOTPRINT</t>
   </si>
   <si>
-    <t xml:space="preserve">т1юла къел</t>
+    <t xml:space="preserve">тӀюла къел</t>
   </si>
   <si>
     <t xml:space="preserve">is т1юла necessary to interpret this as a footprint?</t>
   </si>
   <si>
-    <t xml:space="preserve">т1юла къелме</t>
+    <t xml:space="preserve">тӀюла къелме</t>
   </si>
   <si>
     <t xml:space="preserve">ПАЛЕЦ НОГИ</t>
@@ -4600,13 +4600,13 @@
     <t xml:space="preserve">FEATHER</t>
   </si>
   <si>
-    <t xml:space="preserve">ппих1яла</t>
+    <t xml:space="preserve">ппихӀяла</t>
   </si>
   <si>
     <t xml:space="preserve">pːiħaˁla</t>
   </si>
   <si>
-    <t xml:space="preserve">ппих1ле</t>
+    <t xml:space="preserve">ппихӀле</t>
   </si>
   <si>
     <t xml:space="preserve">pːiħle</t>
@@ -4648,10 +4648,10 @@
     <t xml:space="preserve">NIPPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ихъ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1ихъме</t>
+    <t xml:space="preserve">тӀихъ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀихъме</t>
   </si>
   <si>
     <t xml:space="preserve">ВЫМЯ</t>
@@ -4684,10 +4684,10 @@
     <t xml:space="preserve">HEART</t>
   </si>
   <si>
-    <t xml:space="preserve">урк1и</t>
-  </si>
-  <si>
-    <t xml:space="preserve">урк1бе</t>
+    <t xml:space="preserve">уркӀи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">уркӀбе</t>
   </si>
   <si>
     <t xml:space="preserve">ЛЕГКОЕ</t>
@@ -4708,10 +4708,10 @@
     <t xml:space="preserve">LIVER</t>
   </si>
   <si>
-    <t xml:space="preserve">дулек1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дулек1ме</t>
+    <t xml:space="preserve">дулекӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дулекӀме</t>
   </si>
   <si>
     <t xml:space="preserve">ПОЧКА</t>
@@ -4720,10 +4720,10 @@
     <t xml:space="preserve">KIDNEY</t>
   </si>
   <si>
-    <t xml:space="preserve">х1юрцец</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1юрцецце</t>
+    <t xml:space="preserve">хӀюрцец</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀюрцецце</t>
   </si>
   <si>
     <t xml:space="preserve">СЕЛЕЗЕНКА</t>
@@ -4744,10 +4744,10 @@
     <t xml:space="preserve">STOMACH</t>
   </si>
   <si>
-    <t xml:space="preserve">к1улт1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1улт1не</t>
+    <t xml:space="preserve">кӀултӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀултӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ЖИВОТ</t>
@@ -4783,7 +4783,7 @@
     <t xml:space="preserve">FAT OF ANIMALS</t>
   </si>
   <si>
-    <t xml:space="preserve">х1юл</t>
+    <t xml:space="preserve">хӀюл</t>
   </si>
   <si>
     <t xml:space="preserve">ЖИРНЫЙ</t>
@@ -4792,7 +4792,7 @@
     <t xml:space="preserve">FAT (ADJ)</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1ерхь(це)</t>
+    <t xml:space="preserve">цӀерхь(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ЯГОДИЦЫ</t>
@@ -4813,10 +4813,10 @@
     <t xml:space="preserve">WOMB</t>
   </si>
   <si>
-    <t xml:space="preserve">дух1нук </t>
-  </si>
-  <si>
-    <t xml:space="preserve">дух1нуке </t>
+    <t xml:space="preserve">духӀнук </t>
+  </si>
+  <si>
+    <t xml:space="preserve">духӀнуке </t>
   </si>
   <si>
     <t xml:space="preserve">ВЛАГАЛИЩЕ</t>
@@ -4837,13 +4837,13 @@
     <t xml:space="preserve">PLACENTA</t>
   </si>
   <si>
-    <t xml:space="preserve">дёх1нуш</t>
+    <t xml:space="preserve">дёхӀнуш</t>
   </si>
   <si>
     <t xml:space="preserve">needs to be checked again</t>
   </si>
   <si>
-    <t xml:space="preserve">дёх1нуше</t>
+    <t xml:space="preserve">дёхӀнуше</t>
   </si>
   <si>
     <t xml:space="preserve">ПУПОВИНА</t>
@@ -4852,10 +4852,10 @@
     <t xml:space="preserve">UMBILICAL CORD</t>
   </si>
   <si>
-    <t xml:space="preserve">зак1улт1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">зак1улт1не</t>
+    <t xml:space="preserve">закӀултӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">закӀултӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ЯИЧКИ МУЖСКИЕ</t>
@@ -4894,7 +4894,7 @@
     <t xml:space="preserve">BREATHE</t>
   </si>
   <si>
-    <t xml:space="preserve">ссих1 бик1вий</t>
+    <t xml:space="preserve">ссихӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">sːiħ ikʼʷij</t>
@@ -4909,7 +4909,7 @@
     <t xml:space="preserve">YAWN</t>
   </si>
   <si>
-    <t xml:space="preserve">гьагь бик1вий</t>
+    <t xml:space="preserve">гьагь бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">КАШЛЯТЬ</t>
@@ -4918,7 +4918,7 @@
     <t xml:space="preserve">COUGH</t>
   </si>
   <si>
-    <t xml:space="preserve">къегь бик1вий</t>
+    <t xml:space="preserve">къегь бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ЧИХАТЬ</t>
@@ -4927,7 +4927,7 @@
     <t xml:space="preserve">SNEEZE</t>
   </si>
   <si>
-    <t xml:space="preserve">пишт1 бик1вий</t>
+    <t xml:space="preserve">пиштӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ПОТЕТЬ</t>
@@ -4990,10 +4990,10 @@
     <t xml:space="preserve">BITE</t>
   </si>
   <si>
-    <t xml:space="preserve">кьац1 биккий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">кьац1 билккий</t>
+    <t xml:space="preserve">кьацӀ биккий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кьацӀ билккий</t>
   </si>
   <si>
     <t xml:space="preserve">ЛИЗАТЬ</t>
@@ -5002,10 +5002,10 @@
     <t xml:space="preserve">LICK</t>
   </si>
   <si>
-    <t xml:space="preserve">ламц1 баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ламц1 биркьий</t>
+    <t xml:space="preserve">ламцӀ баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ламцӀ биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">СЛЮНА</t>
@@ -5020,7 +5020,7 @@
     <t xml:space="preserve">This word fits context 1 (‘there is saliva in the mouth’).</t>
   </si>
   <si>
-    <t xml:space="preserve">шу1т1а</t>
+    <t xml:space="preserve">шуӀтӀа</t>
   </si>
   <si>
     <t xml:space="preserve">This word fits context 2 (‘I spit out saliva’).</t>
@@ -5041,7 +5041,7 @@
     <t xml:space="preserve">SNORE</t>
   </si>
   <si>
-    <t xml:space="preserve">хёрх бик1вий</t>
+    <t xml:space="preserve">хёрх бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">СНОВИДЕНИЕ</t>
@@ -5113,7 +5113,7 @@
     <t xml:space="preserve">COPULATE</t>
   </si>
   <si>
-    <t xml:space="preserve">бу1х1ий</t>
+    <t xml:space="preserve">буӀхӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ДРОЖАТЬ (ОТ ХОЛОДА)</t>
@@ -5128,7 +5128,7 @@
     <t xml:space="preserve">shiver strongly</t>
   </si>
   <si>
-    <t xml:space="preserve">гаргар бик1вий</t>
+    <t xml:space="preserve">гаргар бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">shiver a little bit</t>
@@ -5146,10 +5146,10 @@
     <t xml:space="preserve">SHUDDER</t>
   </si>
   <si>
-    <t xml:space="preserve">урк1 бухъий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">урк1 булхъий</t>
+    <t xml:space="preserve">уркӀ бухъий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">уркӀ булхъий</t>
   </si>
   <si>
     <t xml:space="preserve">МЫТЬСЯ</t>
@@ -5194,7 +5194,7 @@
     <t xml:space="preserve">PREGNANT</t>
   </si>
   <si>
-    <t xml:space="preserve">к1улт1нарце</t>
+    <t xml:space="preserve">кӀултӀнарце</t>
   </si>
   <si>
     <t xml:space="preserve">ЖИТЬ, СУЩЕСТВОВАТЬ</t>
@@ -5215,7 +5215,7 @@
     <t xml:space="preserve">ALIVE</t>
   </si>
   <si>
-    <t xml:space="preserve">миц1ирце</t>
+    <t xml:space="preserve">мицӀирце</t>
   </si>
   <si>
     <t xml:space="preserve">УМИРАТЬ</t>
@@ -5224,13 +5224,13 @@
     <t xml:space="preserve">DIE</t>
   </si>
   <si>
-    <t xml:space="preserve">бебч1ий</t>
+    <t xml:space="preserve">бебчӀий</t>
   </si>
   <si>
     <t xml:space="preserve">bebčʼij</t>
   </si>
   <si>
-    <t xml:space="preserve">бубч1ий</t>
+    <t xml:space="preserve">бубчӀий</t>
   </si>
   <si>
     <t xml:space="preserve">bubčʼij</t>
@@ -5242,7 +5242,7 @@
     <t xml:space="preserve">DEAD</t>
   </si>
   <si>
-    <t xml:space="preserve">бебч1ибце</t>
+    <t xml:space="preserve">бебчӀибце</t>
   </si>
   <si>
     <t xml:space="preserve">УБИВАТЬ</t>
@@ -5353,10 +5353,10 @@
     <t xml:space="preserve">TOMBSTONE</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1елтта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ц1елтне</t>
+    <t xml:space="preserve">цӀелтта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цӀелтне</t>
   </si>
   <si>
     <t xml:space="preserve">СИЛЬНЫЙ</t>
@@ -5365,7 +5365,7 @@
     <t xml:space="preserve">STRONG</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1акьце</t>
+    <t xml:space="preserve">цӀакьце</t>
   </si>
   <si>
     <t xml:space="preserve">ЗДОРОВЫЙ</t>
@@ -5386,7 +5386,7 @@
     <t xml:space="preserve">SICK</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ярккаце</t>
+    <t xml:space="preserve">гӀярккаце</t>
   </si>
   <si>
     <t xml:space="preserve">зяипце</t>
@@ -5446,10 +5446,10 @@
     <t xml:space="preserve">ццумазризе</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1ирисан</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ц1ирисанте</t>
+    <t xml:space="preserve">цӀирисан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цӀирисанте</t>
   </si>
   <si>
     <t xml:space="preserve">МОЗОЛЬ</t>
@@ -5458,13 +5458,13 @@
     <t xml:space="preserve">BLISTER</t>
   </si>
   <si>
-    <t xml:space="preserve">пёшшук1</t>
+    <t xml:space="preserve">пёшшукӀ</t>
   </si>
   <si>
     <t xml:space="preserve">волдырь пузырь</t>
   </si>
   <si>
-    <t xml:space="preserve">пёшшук1е</t>
+    <t xml:space="preserve">пёшшукӀе</t>
   </si>
   <si>
     <t xml:space="preserve">ОПУХОЛЬ</t>
@@ -5527,10 +5527,10 @@
     <t xml:space="preserve">SCAR</t>
   </si>
   <si>
-    <t xml:space="preserve">х1ёна</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1ёнбе</t>
+    <t xml:space="preserve">хӀёна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀёнбе</t>
   </si>
   <si>
     <t xml:space="preserve">БОЛЕТЬ (О ЧАСТИ ТЕЛА)</t>
@@ -5548,10 +5548,10 @@
     <t xml:space="preserve">HEAL (TR)</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ях1 баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ях1 биркьий</t>
+    <t xml:space="preserve">гӀяхӀ баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяхӀ биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ЯД</t>
@@ -5611,7 +5611,7 @@
     <t xml:space="preserve">BALD</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ямч1ун(це)</t>
+    <t xml:space="preserve">гӀямчӀун(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ХРОМОЙ</t>
@@ -5620,7 +5620,7 @@
     <t xml:space="preserve">LAME</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1икь бик1ван</t>
+    <t xml:space="preserve">цӀикь бикӀван</t>
   </si>
   <si>
     <t xml:space="preserve">ХРОМАТЬ</t>
@@ -5629,7 +5629,7 @@
     <t xml:space="preserve">GO LIMPING</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1икь бик1вий</t>
+    <t xml:space="preserve">цӀикь бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ГЛУХОЙ</t>
@@ -5638,7 +5638,7 @@
     <t xml:space="preserve">DEAF</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ёнц1(це)</t>
+    <t xml:space="preserve">гӀёнцӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">НЕМОЙ</t>
@@ -5647,7 +5647,7 @@
     <t xml:space="preserve">MUTE</t>
   </si>
   <si>
-    <t xml:space="preserve">гъай бик1вий абирхван</t>
+    <t xml:space="preserve">гъай бикӀвий абирхван</t>
   </si>
   <si>
     <t xml:space="preserve">СЛЕПОЙ</t>
@@ -5674,7 +5674,7 @@
     <t xml:space="preserve">NAKED</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ямк1у(це)</t>
+    <t xml:space="preserve">чӀямкӀу(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ЕСТЬ (ПЕРЕХ.)</t>
@@ -5731,10 +5731,10 @@
     <t xml:space="preserve">RIPEN</t>
   </si>
   <si>
-    <t xml:space="preserve">берц1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">буц1ий</t>
+    <t xml:space="preserve">берцӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">буцӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ГНИТЬ</t>
@@ -5764,7 +5764,7 @@
     <t xml:space="preserve">MILDEW</t>
   </si>
   <si>
-    <t xml:space="preserve">шамак1</t>
+    <t xml:space="preserve">шамакӀ</t>
   </si>
   <si>
     <t xml:space="preserve">ВЯНУТЬ (О ЦВЕТКЕ)</t>
@@ -5782,7 +5782,7 @@
     <t xml:space="preserve">шшул бяхъий</t>
   </si>
   <si>
-    <t xml:space="preserve">шшул бу1рхъий</t>
+    <t xml:space="preserve">шшул буӀрхъий</t>
   </si>
   <si>
     <t xml:space="preserve">ПИТЬ</t>
@@ -5830,10 +5830,10 @@
     <t xml:space="preserve">SUCK (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ёп баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ч1ёп биркьий</t>
+    <t xml:space="preserve">чӀёп баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чӀёп биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ЖЕВАТЬ</t>
@@ -5842,10 +5842,10 @@
     <t xml:space="preserve">CHEW (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ям баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ч1ям биркьий</t>
+    <t xml:space="preserve">чӀям баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чӀям биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ГЛОТАТЬ</t>
@@ -5854,22 +5854,22 @@
     <t xml:space="preserve">SWALLOW (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">кьу1рт1агъий</t>
+    <t xml:space="preserve">кьуӀртӀагъий</t>
   </si>
   <si>
     <t xml:space="preserve">this is German: schlucken</t>
   </si>
   <si>
-    <t xml:space="preserve">кьу1рт1игъий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хьурт1агъий</t>
+    <t xml:space="preserve">кьуӀртӀигъий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хьуртӀагъий</t>
   </si>
   <si>
     <t xml:space="preserve">this is German: verschlucken</t>
   </si>
   <si>
-    <t xml:space="preserve">хьурт1игъий</t>
+    <t xml:space="preserve">хьуртӀигъий</t>
   </si>
   <si>
     <t xml:space="preserve">ГРЫЗТЬ</t>
@@ -5878,7 +5878,7 @@
     <t xml:space="preserve">GNAW (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">хъимс бик1вий</t>
+    <t xml:space="preserve">хъимс бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">this fits the squirrel, but not the dog (like in German knabbern) ALSO: aspect?</t>
@@ -5959,10 +5959,10 @@
     <t xml:space="preserve">CAULDRON (METAL)</t>
   </si>
   <si>
-    <t xml:space="preserve">х1яшак</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1яшукке</t>
+    <t xml:space="preserve">хӀяшак</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀяшукке</t>
   </si>
   <si>
     <t xml:space="preserve">ГОРШОК (ГЛИНЯНЫЙ)</t>
@@ -5995,10 +5995,10 @@
     <t xml:space="preserve">PLATE</t>
   </si>
   <si>
-    <t xml:space="preserve">хат1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хат1не</t>
+    <t xml:space="preserve">хатӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хатӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ПОСУДА</t>
@@ -6007,7 +6007,7 @@
     <t xml:space="preserve">DISHES</t>
   </si>
   <si>
-    <t xml:space="preserve">т1алях1не</t>
+    <t xml:space="preserve">тӀаляхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">КУВШИН ДЛЯ НОШЕНИЯ ВОДЫ</t>
@@ -6028,10 +6028,10 @@
     <t xml:space="preserve">SPOON</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ац1ул</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1ац1ле</t>
+    <t xml:space="preserve">кӀацӀул</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀацӀле</t>
   </si>
   <si>
     <t xml:space="preserve">ВИЛКА</t>
@@ -6040,10 +6040,10 @@
     <t xml:space="preserve">FORK</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ч1уле</t>
+    <t xml:space="preserve">чӀала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чӀуле</t>
   </si>
   <si>
     <t xml:space="preserve">ПОЛОВНИК</t>
@@ -6052,10 +6052,10 @@
     <t xml:space="preserve">LADLE</t>
   </si>
   <si>
-    <t xml:space="preserve">нергъ гьерц1ан</t>
-  </si>
-  <si>
-    <t xml:space="preserve">нергъ гьерц1анте</t>
+    <t xml:space="preserve">нергъ гьерцӀан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">нергъ гьерцӀанте</t>
   </si>
   <si>
     <t xml:space="preserve">ШУМОВКА</t>
@@ -6079,7 +6079,7 @@
     <t xml:space="preserve">сяъ</t>
   </si>
   <si>
-    <t xml:space="preserve">су1ъре</t>
+    <t xml:space="preserve">суӀъре</t>
   </si>
   <si>
     <t xml:space="preserve">СИТО</t>
@@ -6100,10 +6100,10 @@
     <t xml:space="preserve">PEEL (TR, OF FRUIT)</t>
   </si>
   <si>
-    <t xml:space="preserve">чирг1ямч1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">чирг1у1мч1ий</t>
+    <t xml:space="preserve">чиргӀямчӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чиргӀуӀмчӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ПРОСЕИВАТЬ</t>
@@ -6166,10 +6166,10 @@
     <t xml:space="preserve">BREAD</t>
   </si>
   <si>
-    <t xml:space="preserve">т1улт1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1улт1е</t>
+    <t xml:space="preserve">тӀултӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀултӀе</t>
   </si>
   <si>
     <t xml:space="preserve">ТОЛОКНО</t>
@@ -6202,16 +6202,16 @@
     <t xml:space="preserve">CHUDU</t>
   </si>
   <si>
-    <t xml:space="preserve">барццик1в</t>
+    <t xml:space="preserve">барццикӀв</t>
   </si>
   <si>
     <t xml:space="preserve">Both words are equally common.</t>
   </si>
   <si>
-    <t xml:space="preserve">барццик1ве</t>
-  </si>
-  <si>
-    <t xml:space="preserve">баркквиц1</t>
+    <t xml:space="preserve">барццикӀве</t>
+  </si>
+  <si>
+    <t xml:space="preserve">баркквицӀ</t>
   </si>
   <si>
     <t xml:space="preserve">ТЕСТО</t>
@@ -6241,7 +6241,7 @@
     <t xml:space="preserve">FLOUR</t>
   </si>
   <si>
-    <t xml:space="preserve">бет1у</t>
+    <t xml:space="preserve">бетӀу</t>
   </si>
   <si>
     <t xml:space="preserve">МОЛОТЬ (МУКУ)</t>
@@ -6310,7 +6310,7 @@
     <t xml:space="preserve">KHINKAL</t>
   </si>
   <si>
-    <t xml:space="preserve">ххинк1</t>
+    <t xml:space="preserve">ххинкӀ</t>
   </si>
   <si>
     <t xml:space="preserve">does this denote the whole dish or just a piece of khinkal?</t>
@@ -6322,7 +6322,7 @@
     <t xml:space="preserve">GRAPE</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ут1и</t>
+    <t xml:space="preserve">тӀутӀи</t>
   </si>
   <si>
     <t xml:space="preserve">ОРЕХ ЛЕСНОЙ</t>
@@ -6358,7 +6358,7 @@
     <t xml:space="preserve">URBECH</t>
   </si>
   <si>
-    <t xml:space="preserve">п1ялц1ик1в</t>
+    <t xml:space="preserve">пӀялцӀикӀв</t>
   </si>
   <si>
     <t xml:space="preserve">ЖИР (КУЛИНАРНЫЙ ПРОДУКТ)</t>
@@ -6640,7 +6640,7 @@
     <t xml:space="preserve">FABRIC</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ямч1и</t>
+    <t xml:space="preserve">чӀямчӀи</t>
   </si>
   <si>
     <t xml:space="preserve">ПРЯСТЬ</t>
@@ -6688,7 +6688,7 @@
     <t xml:space="preserve">LOOM</t>
   </si>
   <si>
-    <t xml:space="preserve">т1амсса биркьан</t>
+    <t xml:space="preserve">тӀамсса биркьан</t>
   </si>
   <si>
     <r>
@@ -6721,7 +6721,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">т1амсса биркьанте</t>
+    <t xml:space="preserve">тӀамсса биркьанте</t>
   </si>
   <si>
     <t xml:space="preserve">OB: I extrapolated the plural</t>
@@ -6787,10 +6787,10 @@
     <t xml:space="preserve">THREAD</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ат1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1ут1ре</t>
+    <t xml:space="preserve">тӀатӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀутӀре</t>
   </si>
   <si>
     <t xml:space="preserve">МОТОК НИТОК</t>
@@ -6799,10 +6799,10 @@
     <t xml:space="preserve">SKEIN</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1ик1ва</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ц1ик1вне</t>
+    <t xml:space="preserve">цӀикӀва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цӀикӀвне</t>
   </si>
   <si>
     <t xml:space="preserve">НАПЕРСТОК</t>
@@ -6811,10 +6811,10 @@
     <t xml:space="preserve">THIMBLE</t>
   </si>
   <si>
-    <t xml:space="preserve">дархизала т1уппугала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дархизала т1уппугле</t>
+    <t xml:space="preserve">дархизала тӀуппугала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дархизала тӀуппугле</t>
   </si>
   <si>
     <t xml:space="preserve">ГРЕБЕНЬ ДЛЯ ШЕРСТИ</t>
@@ -6832,10 +6832,10 @@
     <t xml:space="preserve">FUR COAT</t>
   </si>
   <si>
-    <t xml:space="preserve">х1яка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1якне</t>
+    <t xml:space="preserve">хӀяка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀякне</t>
   </si>
   <si>
     <t xml:space="preserve">БУРКА</t>
@@ -6955,10 +6955,10 @@
     <t xml:space="preserve">BELT</t>
   </si>
   <si>
-    <t xml:space="preserve">ппяг1ни</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ппяг1нуппе</t>
+    <t xml:space="preserve">ппягӀни</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ппягӀнуппе</t>
   </si>
   <si>
     <t xml:space="preserve">РЕМЕШОК</t>
@@ -6979,10 +6979,10 @@
     <t xml:space="preserve">MITTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">кват1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">кват1не</t>
+    <t xml:space="preserve">кватӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кватӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ПЛАТОК ЖЕНСКИЙ</t>
@@ -6991,10 +6991,10 @@
     <t xml:space="preserve">HEADSCARF</t>
   </si>
   <si>
-    <t xml:space="preserve">ккат1и</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ккат1не</t>
+    <t xml:space="preserve">ккатӀи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ккатӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ЧУХТА</t>
@@ -7003,10 +7003,10 @@
     <t xml:space="preserve">CHUKHTA</t>
   </si>
   <si>
-    <t xml:space="preserve">чук1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">чук1ме</t>
+    <t xml:space="preserve">чукӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чукӀме</t>
   </si>
   <si>
     <t xml:space="preserve">КАРМАН</t>
@@ -7051,10 +7051,10 @@
     <t xml:space="preserve">RING</t>
   </si>
   <si>
-    <t xml:space="preserve">т1уппугала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1уппугле</t>
+    <t xml:space="preserve">тӀуппугала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀуппугле</t>
   </si>
   <si>
     <t xml:space="preserve">БРАСЛЕТ</t>
@@ -7099,10 +7099,10 @@
     <t xml:space="preserve">EARRING</t>
   </si>
   <si>
-    <t xml:space="preserve">урц1ала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">урц1ле</t>
+    <t xml:space="preserve">урцӀала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">урцӀле</t>
   </si>
   <si>
     <t xml:space="preserve">ТАТУИРОВКА</t>
@@ -7159,22 +7159,22 @@
     <t xml:space="preserve">RAZOR</t>
   </si>
   <si>
-    <t xml:space="preserve">дяг1 иссан</t>
+    <t xml:space="preserve">дягӀ иссан</t>
   </si>
   <si>
     <t xml:space="preserve">safety razor</t>
   </si>
   <si>
-    <t xml:space="preserve">дяг1 иссанте</t>
-  </si>
-  <si>
-    <t xml:space="preserve">мут1рус</t>
+    <t xml:space="preserve">дягӀ иссанте</t>
+  </si>
+  <si>
+    <t xml:space="preserve">мутӀрус</t>
   </si>
   <si>
     <t xml:space="preserve">unsafe razor</t>
   </si>
   <si>
-    <t xml:space="preserve">мут1руссе</t>
+    <t xml:space="preserve">мутӀруссе</t>
   </si>
   <si>
     <t xml:space="preserve">БРИТЬ</t>
@@ -7207,10 +7207,10 @@
     <t xml:space="preserve">SOAP</t>
   </si>
   <si>
-    <t xml:space="preserve">ссях1бан</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ссях1бунте</t>
+    <t xml:space="preserve">ссяхӀбан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ссяхӀбунте</t>
   </si>
   <si>
     <t xml:space="preserve">ЗЕРКАЛО</t>
@@ -7219,10 +7219,10 @@
     <t xml:space="preserve">MIRROR</t>
   </si>
   <si>
-    <t xml:space="preserve">лях1имц1ала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">лях1имц1не</t>
+    <t xml:space="preserve">ляхӀимцӀала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ляхӀимцӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ДОМ</t>
@@ -7252,10 +7252,10 @@
     <t xml:space="preserve">RUIN</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ёт1 кабижибце</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ёт1 кадижибте</t>
+    <t xml:space="preserve">гӀётӀ кабижибце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀётӀ кадижибте</t>
   </si>
   <si>
     <t xml:space="preserve">ДВОР</t>
@@ -7369,10 +7369,10 @@
     <t xml:space="preserve">WINDOW</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ями</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ямре</t>
+    <t xml:space="preserve">гӀями</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀямре</t>
   </si>
   <si>
     <t xml:space="preserve">ПОЛ (ЗЕМЛЯНОЙ)</t>
@@ -7381,7 +7381,7 @@
     <t xml:space="preserve">FLOOR</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1ябар</t>
+    <t xml:space="preserve">чӀябар</t>
   </si>
   <si>
     <t xml:space="preserve">ПОТОЛОК</t>
@@ -7453,10 +7453,10 @@
     <t xml:space="preserve">CHIMNEY</t>
   </si>
   <si>
-    <t xml:space="preserve">кьяп1и</t>
-  </si>
-  <si>
-    <t xml:space="preserve">кьяп1не</t>
+    <t xml:space="preserve">кьяпӀи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кьяпӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ЛЕСТНИЦА</t>
@@ -7489,10 +7489,10 @@
     <t xml:space="preserve">PILLOW</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ялихьан</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ялихьне</t>
+    <t xml:space="preserve">гӀялихьан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀялихьне</t>
   </si>
   <si>
     <t xml:space="preserve">ОДЕЯЛО</t>
@@ -7555,10 +7555,10 @@
     <t xml:space="preserve">TABLE</t>
   </si>
   <si>
-    <t xml:space="preserve">уст1ул</t>
-  </si>
-  <si>
-    <t xml:space="preserve">уст1улте</t>
+    <t xml:space="preserve">устӀул</t>
+  </si>
+  <si>
+    <t xml:space="preserve">устӀулте</t>
   </si>
   <si>
     <t xml:space="preserve">ЛАМПА</t>
@@ -7642,10 +7642,10 @@
     <t xml:space="preserve">WALLPOST</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ал</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1уле</t>
+    <t xml:space="preserve">тӀал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀуле</t>
   </si>
   <si>
     <t xml:space="preserve">ДОСКА</t>
@@ -7777,7 +7777,7 @@
     <t xml:space="preserve">укъий</t>
   </si>
   <si>
-    <t xml:space="preserve">гьабит1ий</t>
+    <t xml:space="preserve">гьабитӀий</t>
   </si>
   <si>
     <t xml:space="preserve">гьабилтий</t>
@@ -7792,10 +7792,10 @@
     <t xml:space="preserve">SPADE</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ат1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1ат1не</t>
+    <t xml:space="preserve">кӀатӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀатӀне</t>
   </si>
   <si>
     <t xml:space="preserve">МОТЫГА</t>
@@ -7888,10 +7888,10 @@
     <t xml:space="preserve">WINNOW</t>
   </si>
   <si>
-    <t xml:space="preserve">сагьаберч1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">сагьадурч1ий</t>
+    <t xml:space="preserve">сагьаберчӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сагьадурчӀий</t>
   </si>
   <si>
     <t xml:space="preserve">СЕМЕНА (СОБИР.)</t>
@@ -8059,7 +8059,7 @@
     <t xml:space="preserve">WHEAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ач1и</t>
+    <t xml:space="preserve">ачӀи</t>
   </si>
   <si>
     <t xml:space="preserve">ЯЧМЕНЬ</t>
@@ -8143,10 +8143,10 @@
     <t xml:space="preserve">ROOT</t>
   </si>
   <si>
-    <t xml:space="preserve">ямх1я</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ямх1не</t>
+    <t xml:space="preserve">ямхӀя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ямхӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ВЕТКА</t>
@@ -8167,10 +8167,10 @@
     <t xml:space="preserve">LEAF</t>
   </si>
   <si>
-    <t xml:space="preserve">к1аппур</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1апре</t>
+    <t xml:space="preserve">кӀаппур</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀапре</t>
   </si>
   <si>
     <t xml:space="preserve">ЦВЕТОК</t>
@@ -8203,10 +8203,10 @@
     <t xml:space="preserve">BUSH</t>
   </si>
   <si>
-    <t xml:space="preserve">къват1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">къват1не</t>
+    <t xml:space="preserve">къватӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">къватӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ДУБ</t>
@@ -8347,7 +8347,7 @@
     <t xml:space="preserve">FRUIT</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1идехь</t>
+    <t xml:space="preserve">цӀидехь</t>
   </si>
   <si>
     <t xml:space="preserve">ЯБЛОКО</t>
@@ -8401,7 +8401,7 @@
     <t xml:space="preserve">PLUM</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1ултми</t>
+    <t xml:space="preserve">цӀултми</t>
   </si>
   <si>
     <t xml:space="preserve">БАРБАРИС</t>
@@ -8488,7 +8488,7 @@
     <t xml:space="preserve">REED</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1их1я</t>
+    <t xml:space="preserve">чӀихӀя</t>
   </si>
   <si>
     <t xml:space="preserve">СОРНЯК</t>
@@ -8497,7 +8497,7 @@
     <t xml:space="preserve">WEED</t>
   </si>
   <si>
-    <t xml:space="preserve">арц1и</t>
+    <t xml:space="preserve">арцӀи</t>
   </si>
   <si>
     <t xml:space="preserve">КОЛЮЧКА</t>
@@ -8533,10 +8533,10 @@
     <t xml:space="preserve">MUSHROOM</t>
   </si>
   <si>
-    <t xml:space="preserve">шайт1анна хъати</t>
-  </si>
-  <si>
-    <t xml:space="preserve">шайт1анна хъатне</t>
+    <t xml:space="preserve">шайтӀанна хъати</t>
+  </si>
+  <si>
+    <t xml:space="preserve">шайтӀанна хъатне</t>
   </si>
   <si>
     <t xml:space="preserve">ДЕЛАТЬ</t>
@@ -8572,10 +8572,10 @@
     <t xml:space="preserve">BEND (TR)</t>
   </si>
   <si>
-    <t xml:space="preserve">балк1ун баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">балк1ун биркьий</t>
+    <t xml:space="preserve">балкӀун баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">балкӀун биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ГНУТЬСЯ</t>
@@ -8584,10 +8584,10 @@
     <t xml:space="preserve">BEND (INTR)</t>
   </si>
   <si>
-    <t xml:space="preserve">балк1ун бихвий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">балк1ун бирхвий</t>
+    <t xml:space="preserve">балкӀун бихвий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">балкӀун бирхвий</t>
   </si>
   <si>
     <t xml:space="preserve">СВЯЗЫВАТЬ (ПРЕДМЕТЫ)</t>
@@ -8632,10 +8632,10 @@
     <t xml:space="preserve">ROPE, CORD</t>
   </si>
   <si>
-    <t xml:space="preserve">т1алим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1алимте</t>
+    <t xml:space="preserve">тӀалим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀалимте</t>
   </si>
   <si>
     <t xml:space="preserve">УЗЕЛ</t>
@@ -8644,10 +8644,10 @@
     <t xml:space="preserve">KNOT (NOUN)</t>
   </si>
   <si>
-    <t xml:space="preserve">кьу1кья</t>
-  </si>
-  <si>
-    <t xml:space="preserve">кьу1кьме</t>
+    <t xml:space="preserve">кьуӀкья</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кьуӀкьме</t>
   </si>
   <si>
     <t xml:space="preserve">БИТЬ, ИЗБИВАТЬ</t>
@@ -8674,7 +8674,7 @@
     <t xml:space="preserve">there is also another verb бургьий   — can be added as excluded with both stems</t>
   </si>
   <si>
-    <t xml:space="preserve">бу1рхъий</t>
+    <t xml:space="preserve">буӀрхъий</t>
   </si>
   <si>
     <t xml:space="preserve">РУБИТЬ</t>
@@ -8842,10 +8842,10 @@
     <t xml:space="preserve">RUB (V, BY HAND)</t>
   </si>
   <si>
-    <t xml:space="preserve">сурк1 баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">сурк1 биркьий</t>
+    <t xml:space="preserve">суркӀ баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">суркӀ биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ЧЕСАТЬ</t>
@@ -8917,13 +8917,13 @@
     <t xml:space="preserve">PULL</t>
   </si>
   <si>
-    <t xml:space="preserve">бит1ач1ий</t>
+    <t xml:space="preserve">битӀачӀий</t>
   </si>
   <si>
     <t xml:space="preserve">bitʼačʼij</t>
   </si>
   <si>
-    <t xml:space="preserve">бит1ич1ий</t>
+    <t xml:space="preserve">битӀичӀий</t>
   </si>
   <si>
     <t xml:space="preserve">bitʼičʼij</t>
@@ -8938,7 +8938,7 @@
     <t xml:space="preserve">хъус бяхъий</t>
   </si>
   <si>
-    <t xml:space="preserve">хъус бу1рхъий</t>
+    <t xml:space="preserve">хъус буӀрхъий</t>
   </si>
   <si>
     <t xml:space="preserve">ВЕШАТЬ</t>
@@ -8971,10 +8971,10 @@
     <t xml:space="preserve">PRESS (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">гъуч1 баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">гъуч1 биркьий</t>
+    <t xml:space="preserve">гъучӀ баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гъучӀ биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ЛИТЬ</t>
@@ -8983,10 +8983,10 @@
     <t xml:space="preserve">POUR (TR, LIQUID)</t>
   </si>
   <si>
-    <t xml:space="preserve">кат1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">керт1ий</t>
+    <t xml:space="preserve">катӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кертӀий</t>
   </si>
   <si>
     <t xml:space="preserve">СЫПАТЬСЯ</t>
@@ -9076,10 +9076,10 @@
     <t xml:space="preserve">TROUGH</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ени</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1енбе</t>
+    <t xml:space="preserve">тӀени</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀенбе</t>
   </si>
   <si>
     <t xml:space="preserve">ТЕСАТЬ</t>
@@ -9100,10 +9100,10 @@
     <t xml:space="preserve">BORE</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ями кажий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1ями каржий</t>
+    <t xml:space="preserve">гӀями кажий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀями каржий</t>
   </si>
   <si>
     <t xml:space="preserve">ПИЛА</t>
@@ -9196,10 +9196,10 @@
     <t xml:space="preserve">TONGS</t>
   </si>
   <si>
-    <t xml:space="preserve">къац1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">къац1не</t>
+    <t xml:space="preserve">къацӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">къацӀне</t>
   </si>
   <si>
     <t xml:space="preserve">КРЕМЕНЬ</t>
@@ -9208,10 +9208,10 @@
     <t xml:space="preserve">FLINT</t>
   </si>
   <si>
-    <t xml:space="preserve">х1яшур</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1яшурме</t>
+    <t xml:space="preserve">хӀяшур</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀяшурме</t>
   </si>
   <si>
     <t xml:space="preserve">ТРУТ</t>
@@ -9325,7 +9325,7 @@
     <t xml:space="preserve">GLASS</t>
   </si>
   <si>
-    <t xml:space="preserve">ссулу1х1и</t>
+    <t xml:space="preserve">ссулуӀхӀи</t>
   </si>
   <si>
     <t xml:space="preserve">ТКАТЬ</t>
@@ -9334,10 +9334,10 @@
     <t xml:space="preserve">WEAVE</t>
   </si>
   <si>
-    <t xml:space="preserve">т1амсса баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1амсса биркьий</t>
+    <t xml:space="preserve">тӀамсса баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀамсса биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">КОРЗИНА</t>
@@ -9346,7 +9346,7 @@
     <t xml:space="preserve">BASKET</t>
   </si>
   <si>
-    <t xml:space="preserve">т1уннехъ</t>
+    <t xml:space="preserve">тӀуннехъ</t>
   </si>
   <si>
     <t xml:space="preserve">СУНДУК</t>
@@ -9373,10 +9373,10 @@
     <t xml:space="preserve">WATERSKIN</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ахьва</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1ахьне</t>
+    <t xml:space="preserve">тӀахьва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀахьне</t>
   </si>
   <si>
     <t xml:space="preserve">МЕШОК</t>
@@ -9397,10 +9397,10 @@
     <t xml:space="preserve">CARPET</t>
   </si>
   <si>
-    <t xml:space="preserve">т1амсса</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1амсне</t>
+    <t xml:space="preserve">тӀамсса</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀамсне</t>
   </si>
   <si>
     <t xml:space="preserve">ПАЛАС (КОВЁР БЕЗ ВОРСА)</t>
@@ -9409,10 +9409,10 @@
     <t xml:space="preserve">MAT</t>
   </si>
   <si>
-    <t xml:space="preserve">к1варч1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1варч1не</t>
+    <t xml:space="preserve">кӀварчӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀварчӀне</t>
   </si>
   <si>
     <t xml:space="preserve">ПАЛАС (ДОРОЖКА)</t>
@@ -9439,7 +9439,7 @@
     <t xml:space="preserve">ROCK (INTR, OF PLANT)</t>
   </si>
   <si>
-    <t xml:space="preserve">гьак1ар бик1вий</t>
+    <t xml:space="preserve">гьакӀар бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">КАЧАТЬ (КОЛЫБЕЛЬ)</t>
@@ -9511,7 +9511,7 @@
     <t xml:space="preserve">DRIP (INTR)</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ат1 бик1вий</t>
+    <t xml:space="preserve">кӀатӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">КАПЛЯ</t>
@@ -9520,10 +9520,10 @@
     <t xml:space="preserve">DROP (N, OF WATER)</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ат1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1ут1ре</t>
+    <t xml:space="preserve">кӀатӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀутӀре</t>
   </si>
   <si>
     <t xml:space="preserve">БРОСАТЬ, КИДАТЬ</t>
@@ -9538,10 +9538,10 @@
     <t xml:space="preserve">ирхьвий</t>
   </si>
   <si>
-    <t xml:space="preserve">лак1 баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">лак1 биркьий</t>
+    <t xml:space="preserve">лакӀ баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">лакӀ биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ЛОВИТЬ (МЯЧ)</t>
@@ -9586,7 +9586,7 @@
     <t xml:space="preserve">SWING (TR, STICK)</t>
   </si>
   <si>
-    <t xml:space="preserve">лях1 бик1вий</t>
+    <t xml:space="preserve">ляхӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ХОДИТЬ (О ЧЕЛОВЕКЕ)</t>
@@ -9619,13 +9619,13 @@
     <t xml:space="preserve">FLY (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ялх1ий</t>
+    <t xml:space="preserve">гӀялхӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ʡaˁlħij</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ях1ий</t>
+    <t xml:space="preserve">гӀяхӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ʡaˁħij</t>
@@ -9649,7 +9649,7 @@
     <t xml:space="preserve">CRAWL (V, OF PERSON)</t>
   </si>
   <si>
-    <t xml:space="preserve">хъус бик1вий</t>
+    <t xml:space="preserve">хъус бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ПРИСЕДАТЬ (НА КОРТОЧКАХ)</t>
@@ -9658,10 +9658,10 @@
     <t xml:space="preserve">CROUCH</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ук1 кабижий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">к1ук1 кабиржий</t>
+    <t xml:space="preserve">кӀукӀ кабижий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кӀукӀ кабиржий</t>
   </si>
   <si>
     <t xml:space="preserve">СКОЛЬЗИТЬ</t>
@@ -9676,7 +9676,7 @@
     <t xml:space="preserve">JUMP, LEAP</t>
   </si>
   <si>
-    <t xml:space="preserve">тях1 бик1вий</t>
+    <t xml:space="preserve">тяхӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ТАНЦЕВАТЬ</t>
@@ -9685,10 +9685,10 @@
     <t xml:space="preserve">DANCE</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яяр биркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1яяр баркьий</t>
+    <t xml:space="preserve">гӀяяр биркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяяр баркьий</t>
   </si>
   <si>
     <t xml:space="preserve">булхъий</t>
@@ -9703,10 +9703,10 @@
     <t xml:space="preserve">DANCE (N)</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яяр</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1яйурте</t>
+    <t xml:space="preserve">гӀяяр</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяйурте</t>
   </si>
   <si>
     <t xml:space="preserve">ШАГ</t>
@@ -9724,7 +9724,7 @@
     <t xml:space="preserve">RUN</t>
   </si>
   <si>
-    <t xml:space="preserve">дуц1 бик1вий</t>
+    <t xml:space="preserve">дуцӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ducʼ bikʼʷij</t>
@@ -10009,10 +10009,10 @@
     <t xml:space="preserve">WHEEL</t>
   </si>
   <si>
-    <t xml:space="preserve">г1у1ла</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1у1лме</t>
+    <t xml:space="preserve">гӀуӀла</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀуӀлме</t>
   </si>
   <si>
     <t xml:space="preserve">ОСЬ</t>
@@ -10033,10 +10033,10 @@
     <t xml:space="preserve">YOKE</t>
   </si>
   <si>
-    <t xml:space="preserve">дук1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дук1ме</t>
+    <t xml:space="preserve">дукӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дукӀме</t>
   </si>
   <si>
     <t xml:space="preserve">НОША</t>
@@ -10105,10 +10105,10 @@
     <t xml:space="preserve">WHIP</t>
   </si>
   <si>
-    <t xml:space="preserve">х1юрчмек</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1юрчмукке</t>
+    <t xml:space="preserve">хӀюрчмек</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀюрчмукке</t>
   </si>
   <si>
     <t xml:space="preserve">СТРЕМЯ</t>
@@ -10126,10 +10126,10 @@
     <t xml:space="preserve">HORSESHOE</t>
   </si>
   <si>
-    <t xml:space="preserve">урчила лут1и</t>
-  </si>
-  <si>
-    <t xml:space="preserve">урчила лут1ме</t>
+    <t xml:space="preserve">урчила лутӀи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">урчила лутӀме</t>
   </si>
   <si>
     <t xml:space="preserve">КОРАБЛЬ</t>
@@ -10243,10 +10243,10 @@
     <t xml:space="preserve">булгий</t>
   </si>
   <si>
-    <t xml:space="preserve">г1у1т1 агъий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1у1т1 игъий</t>
+    <t xml:space="preserve">гӀуӀтӀ агъий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀуӀтӀ игъий</t>
   </si>
   <si>
     <t xml:space="preserve">ИСКАТЬ</t>
@@ -10255,10 +10255,10 @@
     <t xml:space="preserve">LOOK FOR</t>
   </si>
   <si>
-    <t xml:space="preserve">къяйц1 бик1вий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">умц1ий</t>
+    <t xml:space="preserve">къяйцӀ бикӀвий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">умцӀий</t>
   </si>
   <si>
     <t xml:space="preserve">НАХОДИТЬ</t>
@@ -10549,7 +10549,7 @@
     <t xml:space="preserve">THING</t>
   </si>
   <si>
-    <t xml:space="preserve">цик1ал</t>
+    <t xml:space="preserve">цикӀал</t>
   </si>
   <si>
     <t xml:space="preserve">is this really used as a noun ‘thing’? it means ‘something’ as far as I know</t>
@@ -10618,16 +10618,16 @@
     <t xml:space="preserve">HALT</t>
   </si>
   <si>
-    <t xml:space="preserve">т1а кабицций</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1а кабирцций</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1аш кабицций</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1аш кабирцций</t>
+    <t xml:space="preserve">тӀа кабицций</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀа кабирцций</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀаш кабицций</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀаш кабирцций</t>
   </si>
   <si>
     <t xml:space="preserve">СТОЯТЬ</t>
@@ -10660,10 +10660,10 @@
     <t xml:space="preserve">GATHER (TR)</t>
   </si>
   <si>
-    <t xml:space="preserve">балц1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">луц1ий</t>
+    <t xml:space="preserve">балцӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">луцӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ПОДНИМАТЬ</t>
@@ -10684,10 +10684,10 @@
     <t xml:space="preserve">INSERT</t>
   </si>
   <si>
-    <t xml:space="preserve">гьиттитач1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">гьиттитич1ий</t>
+    <t xml:space="preserve">гьиттитачӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гьиттитичӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ПРИВЯЗЫВАТЬ</t>
@@ -10798,10 +10798,10 @@
     <t xml:space="preserve">COVER</t>
   </si>
   <si>
-    <t xml:space="preserve">бяг1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бялг1ий</t>
+    <t xml:space="preserve">бягӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бялгӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ПРЯТАТЬ</t>
@@ -10816,10 +10816,10 @@
     <t xml:space="preserve">гурбиршший</t>
   </si>
   <si>
-    <t xml:space="preserve">дяг1яна бяркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дяг1яна биркьий</t>
+    <t xml:space="preserve">дягӀяна бяркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дягӀяна биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ПРЯТЯТЬСЯ</t>
@@ -10828,10 +10828,10 @@
     <t xml:space="preserve">HIDE (INTR)</t>
   </si>
   <si>
-    <t xml:space="preserve">дяг1яна бихвий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дяг1яна бирхвий</t>
+    <t xml:space="preserve">дягӀяна бихвий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дягӀяна бирхвий</t>
   </si>
   <si>
     <t xml:space="preserve">ВЫСОКИЙ</t>
@@ -10870,13 +10870,13 @@
     <t xml:space="preserve">BOTTOM (N)</t>
   </si>
   <si>
-    <t xml:space="preserve">лут1и</t>
-  </si>
-  <si>
-    <t xml:space="preserve">лут1ме</t>
-  </si>
-  <si>
-    <t xml:space="preserve">лут1илццеб</t>
+    <t xml:space="preserve">лутӀи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">лутӀме</t>
+  </si>
+  <si>
+    <t xml:space="preserve">лутӀилццеб</t>
   </si>
   <si>
     <t xml:space="preserve">КОНЧИК, ОСТРИЕ</t>
@@ -10954,10 +10954,10 @@
     <t xml:space="preserve">GROW</t>
   </si>
   <si>
-    <t xml:space="preserve">бач1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бич1ий</t>
+    <t xml:space="preserve">бачӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бичӀий</t>
   </si>
   <si>
     <t xml:space="preserve">МЕРИТЬ</t>
@@ -10972,7 +10972,7 @@
     <t xml:space="preserve">GREAT SPAN</t>
   </si>
   <si>
-    <t xml:space="preserve">ч1им</t>
+    <t xml:space="preserve">чӀим</t>
   </si>
   <si>
     <t xml:space="preserve">ПЯДЬ МАЛАЯ</t>
@@ -10999,7 +10999,7 @@
     <t xml:space="preserve">SMALL</t>
   </si>
   <si>
-    <t xml:space="preserve">ник1а(це)</t>
+    <t xml:space="preserve">никӀа(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ДЛИННЫЙ</t>
@@ -11020,7 +11020,7 @@
     <t xml:space="preserve">SHORT</t>
   </si>
   <si>
-    <t xml:space="preserve">кут1(це)</t>
+    <t xml:space="preserve">кутӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">kutʼ</t>
@@ -11029,7 +11029,7 @@
     <t xml:space="preserve">Both words are equally used.</t>
   </si>
   <si>
-    <t xml:space="preserve">къант1(це)</t>
+    <t xml:space="preserve">къантӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">qːantʼ</t>
@@ -11071,7 +11071,7 @@
     <t xml:space="preserve">baˁršu</t>
   </si>
   <si>
-    <t xml:space="preserve">бу1ц(це)</t>
+    <t xml:space="preserve">буӀц(це)</t>
   </si>
   <si>
     <t xml:space="preserve">buˁc</t>
@@ -11083,7 +11083,7 @@
     <t xml:space="preserve">THIN</t>
   </si>
   <si>
-    <t xml:space="preserve">гъвирц1(це)</t>
+    <t xml:space="preserve">гъвирцӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ГЛУБОКИЙ</t>
@@ -11101,7 +11101,7 @@
     <t xml:space="preserve">SHALLOW</t>
   </si>
   <si>
-    <t xml:space="preserve">бимг1ян(це)</t>
+    <t xml:space="preserve">бимгӀян(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ПЛОСКИЙ</t>
@@ -11110,7 +11110,7 @@
     <t xml:space="preserve">FLAT</t>
   </si>
   <si>
-    <t xml:space="preserve">бук1ул(це)</t>
+    <t xml:space="preserve">букӀул(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ПРЯМОЙ</t>
@@ -11137,7 +11137,7 @@
     <t xml:space="preserve">CROOKED</t>
   </si>
   <si>
-    <t xml:space="preserve">балк1ун(це)</t>
+    <t xml:space="preserve">балкӀун(це)</t>
   </si>
   <si>
     <t xml:space="preserve">КРЮК</t>
@@ -11293,7 +11293,7 @@
     <t xml:space="preserve">TWO</t>
   </si>
   <si>
-    <t xml:space="preserve">к1вел</t>
+    <t xml:space="preserve">кӀвел</t>
   </si>
   <si>
     <t xml:space="preserve">kʼʷel</t>
@@ -11305,7 +11305,7 @@
     <t xml:space="preserve">THREE</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ябал</t>
+    <t xml:space="preserve">гӀябал</t>
   </si>
   <si>
     <t xml:space="preserve">ʡaˁbal</t>
@@ -11368,7 +11368,7 @@
     <t xml:space="preserve">NINE</t>
   </si>
   <si>
-    <t xml:space="preserve">урч1емал</t>
+    <t xml:space="preserve">урчӀемал</t>
   </si>
   <si>
     <t xml:space="preserve">ДЕСЯТЬ</t>
@@ -11377,7 +11377,7 @@
     <t xml:space="preserve">TEN</t>
   </si>
   <si>
-    <t xml:space="preserve">вец1ал</t>
+    <t xml:space="preserve">вецӀал</t>
   </si>
   <si>
     <t xml:space="preserve">ОДИННАДЦАТЬ</t>
@@ -11386,7 +11386,7 @@
     <t xml:space="preserve">ELEVEN</t>
   </si>
   <si>
-    <t xml:space="preserve">вец1ну цара</t>
+    <t xml:space="preserve">вецӀну цара</t>
   </si>
   <si>
     <t xml:space="preserve">ДВЕНАДЦАТЬ</t>
@@ -11395,7 +11395,7 @@
     <t xml:space="preserve">TWELVE</t>
   </si>
   <si>
-    <t xml:space="preserve">вец1ну к1вира</t>
+    <t xml:space="preserve">вецӀну кӀвира</t>
   </si>
   <si>
     <t xml:space="preserve">ДВАДЦАТЬ</t>
@@ -11413,7 +11413,7 @@
     <t xml:space="preserve">THIRTY</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ябц1ал</t>
+    <t xml:space="preserve">гӀябцӀал</t>
   </si>
   <si>
     <t xml:space="preserve">СТО</t>
@@ -11458,7 +11458,7 @@
     <t xml:space="preserve">SECOND</t>
   </si>
   <si>
-    <t xml:space="preserve">к1виъибил</t>
+    <t xml:space="preserve">кӀвиъибил</t>
   </si>
   <si>
     <t xml:space="preserve">СЧИТАТЬ</t>
@@ -11518,7 +11518,7 @@
     <t xml:space="preserve">VERY</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1акьле</t>
+    <t xml:space="preserve">цӀакьле</t>
   </si>
   <si>
     <t xml:space="preserve">МАЛО</t>
@@ -11533,7 +11533,7 @@
     <t xml:space="preserve">FULL</t>
   </si>
   <si>
-    <t xml:space="preserve">биц1иб(це)</t>
+    <t xml:space="preserve">бицӀиб(це)</t>
   </si>
   <si>
     <t xml:space="preserve">СЫТЫЙ</t>
@@ -11551,7 +11551,7 @@
     <t xml:space="preserve">FILL (INTR)</t>
   </si>
   <si>
-    <t xml:space="preserve">бирц1ий</t>
+    <t xml:space="preserve">бирцӀий</t>
   </si>
   <si>
     <t xml:space="preserve">НАПОЛНЯТЬ</t>
@@ -11566,7 +11566,7 @@
     <t xml:space="preserve">EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">бац1(це)</t>
+    <t xml:space="preserve">бацӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">КУСОК</t>
@@ -11575,10 +11575,10 @@
     <t xml:space="preserve">PIECE</t>
   </si>
   <si>
-    <t xml:space="preserve">бут1а</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бут1нe</t>
+    <t xml:space="preserve">бутӀа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бутӀнe</t>
   </si>
   <si>
     <t xml:space="preserve">ПОЛОВИНА</t>
@@ -11671,13 +11671,13 @@
     <t xml:space="preserve">BEGIN (INTR)</t>
   </si>
   <si>
-    <t xml:space="preserve">баъач1ий</t>
+    <t xml:space="preserve">баъачӀий</t>
   </si>
   <si>
     <t xml:space="preserve">All three verbs are equally used.</t>
   </si>
   <si>
-    <t xml:space="preserve">баъич1ий</t>
+    <t xml:space="preserve">баъичӀий</t>
   </si>
   <si>
     <t xml:space="preserve">баъашший</t>
@@ -11749,7 +11749,7 @@
     <t xml:space="preserve">SOON</t>
   </si>
   <si>
-    <t xml:space="preserve">ниик1алла гьитти</t>
+    <t xml:space="preserve">ниикӀалла гьитти</t>
   </si>
   <si>
     <t xml:space="preserve">ДОЛГО</t>
@@ -11806,7 +11806,7 @@
     <t xml:space="preserve">MORNING</t>
   </si>
   <si>
-    <t xml:space="preserve">ччяг1ялла</t>
+    <t xml:space="preserve">ччягӀялла</t>
   </si>
   <si>
     <t xml:space="preserve">This is an adverb ‘in the morning’ no noun ‘morning’.</t>
@@ -11848,7 +11848,7 @@
     <t xml:space="preserve">TOMORROW</t>
   </si>
   <si>
-    <t xml:space="preserve">ччяг1ял</t>
+    <t xml:space="preserve">ччягӀял</t>
   </si>
   <si>
     <t xml:space="preserve">ПОСЛЕЗАВТРА</t>
@@ -11887,10 +11887,10 @@
     <t xml:space="preserve">HOUR</t>
   </si>
   <si>
-    <t xml:space="preserve">ссяг1ят</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ссяг1ёте</t>
+    <t xml:space="preserve">ссягӀят</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ссягӀёте</t>
   </si>
   <si>
     <t xml:space="preserve">НЕДЕЛЯ</t>
@@ -11899,10 +11899,10 @@
     <t xml:space="preserve">WEEK</t>
   </si>
   <si>
-    <t xml:space="preserve">жумяг1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">жумяг1е</t>
+    <t xml:space="preserve">жумягӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">жумягӀе</t>
   </si>
   <si>
     <t xml:space="preserve">МЕСЯЦ</t>
@@ -11947,7 +11947,7 @@
     <t xml:space="preserve">NEXT YEAR</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1ил дус</t>
+    <t xml:space="preserve">цӀил дус</t>
   </si>
   <si>
     <t xml:space="preserve">ЗИМА</t>
@@ -12001,7 +12001,7 @@
     <t xml:space="preserve">SMELL (TR)</t>
   </si>
   <si>
-    <t xml:space="preserve">кквяг1 ирччий</t>
+    <t xml:space="preserve">кквягӀ ирччий</t>
   </si>
   <si>
     <t xml:space="preserve">There is no intr. verb ‘to smell’, only the noun ‘smell’. ‘X smells good’ is translated as ‘X has a good smell’.</t>
@@ -12013,10 +12013,10 @@
     <t xml:space="preserve">SMELL</t>
   </si>
   <si>
-    <t xml:space="preserve">кквяг1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1ем</t>
+    <t xml:space="preserve">кквягӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀем</t>
   </si>
   <si>
     <t xml:space="preserve">запах, вкус</t>
@@ -12067,7 +12067,7 @@
     <t xml:space="preserve">SOUR</t>
   </si>
   <si>
-    <t xml:space="preserve">кьамц1(це)</t>
+    <t xml:space="preserve">кьамцӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">СЛЫШАТЬ</t>
@@ -12076,13 +12076,13 @@
     <t xml:space="preserve">HEAR</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ам бакьий</t>
+    <t xml:space="preserve">тӀам бакьий</t>
   </si>
   <si>
     <t xml:space="preserve">tʼam baqʼij</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ам бикьий</t>
+    <t xml:space="preserve">тӀам бикьий</t>
   </si>
   <si>
     <t xml:space="preserve">tʼam biqʼij</t>
@@ -12094,7 +12094,7 @@
     <t xml:space="preserve">LISTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">гулик1ий</t>
+    <t xml:space="preserve">гуликӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ГОЛОС</t>
@@ -12103,10 +12103,10 @@
     <t xml:space="preserve">VOICE</t>
   </si>
   <si>
-    <t xml:space="preserve">т1ама</t>
-  </si>
-  <si>
-    <t xml:space="preserve">т1амре</t>
+    <t xml:space="preserve">тӀама</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тӀамре</t>
   </si>
   <si>
     <t xml:space="preserve">ГРОМКИЙ</t>
@@ -12145,13 +12145,13 @@
     <t xml:space="preserve">LOOK</t>
   </si>
   <si>
-    <t xml:space="preserve">эр бик1вий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">эр бурч1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">эр берч1ий</t>
+    <t xml:space="preserve">эр бикӀвий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">эр бурчӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">эр берчӀий</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛЫЙ</t>
@@ -12160,7 +12160,7 @@
     <t xml:space="preserve">WHITE</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1уб(це)</t>
+    <t xml:space="preserve">цӀуб(це)</t>
   </si>
   <si>
     <t xml:space="preserve">cʼub</t>
@@ -12172,7 +12172,7 @@
     <t xml:space="preserve">BLACK</t>
   </si>
   <si>
-    <t xml:space="preserve">ц1уттар(це)</t>
+    <t xml:space="preserve">цӀуттар(це)</t>
   </si>
   <si>
     <t xml:space="preserve">cʼutːar</t>
@@ -12184,7 +12184,7 @@
     <t xml:space="preserve">RED</t>
   </si>
   <si>
-    <t xml:space="preserve">ит1ин(це)</t>
+    <t xml:space="preserve">итӀин(це)</t>
   </si>
   <si>
     <t xml:space="preserve">itʼin</t>
@@ -12196,7 +12196,7 @@
     <t xml:space="preserve">BLUE</t>
   </si>
   <si>
-    <t xml:space="preserve">хьанц1(це)</t>
+    <t xml:space="preserve">хьанцӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ЗЕЛЁНЫЙ</t>
@@ -12262,7 +12262,7 @@
     <t xml:space="preserve">HARD</t>
   </si>
   <si>
-    <t xml:space="preserve">к1ант1и(це)</t>
+    <t xml:space="preserve">кӀантӀи(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ГЛАДКИЙ</t>
@@ -12277,7 +12277,7 @@
     <t xml:space="preserve">SHARP</t>
   </si>
   <si>
-    <t xml:space="preserve">лягъу1н(це)</t>
+    <t xml:space="preserve">лягъуӀн(це)</t>
   </si>
   <si>
     <t xml:space="preserve">laˁʁuˁn</t>
@@ -12301,7 +12301,7 @@
     <t xml:space="preserve">DENSE</t>
   </si>
   <si>
-    <t xml:space="preserve">къут1а(це)</t>
+    <t xml:space="preserve">къутӀа(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ЖИДКИЙ</t>
@@ -12328,7 +12328,7 @@
     <t xml:space="preserve">LIGHT (IN WEIGHT)</t>
   </si>
   <si>
-    <t xml:space="preserve">дек1в(це)</t>
+    <t xml:space="preserve">декӀв(це)</t>
   </si>
   <si>
     <t xml:space="preserve">dekʼʷ</t>
@@ -12349,7 +12349,7 @@
     <t xml:space="preserve">DRY</t>
   </si>
   <si>
-    <t xml:space="preserve">бях1ун(це)</t>
+    <t xml:space="preserve">бяхӀун(це)</t>
   </si>
   <si>
     <t xml:space="preserve">baˁħunce</t>
@@ -12361,7 +12361,7 @@
     <t xml:space="preserve">HOT</t>
   </si>
   <si>
-    <t xml:space="preserve">буц1ар(це)</t>
+    <t xml:space="preserve">буцӀар(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ТЁПЛЫЙ</t>
@@ -12418,7 +12418,7 @@
     <t xml:space="preserve">LAUGH</t>
   </si>
   <si>
-    <t xml:space="preserve">х1ях1я бик1вий</t>
+    <t xml:space="preserve">хӀяхӀя бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ħaˁħaˁ bikʼʷij</t>
@@ -12430,7 +12430,7 @@
     <t xml:space="preserve">SMILE</t>
   </si>
   <si>
-    <t xml:space="preserve">гъигъ бик1вий</t>
+    <t xml:space="preserve">гъигъ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">РАДОВАТЬСЯ</t>
@@ -12451,16 +12451,16 @@
     <t xml:space="preserve">PLAY (TR)</t>
   </si>
   <si>
-    <t xml:space="preserve">х1язле кайжий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1язле кабижий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бу1мг1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">х1язтал биркьий</t>
+    <t xml:space="preserve">хӀязле кайжий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀязле кабижий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">буӀмгӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хӀязтал биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">This is an antipassive construction which cannot be used with intransitive verbs.</t>
@@ -12562,7 +12562,7 @@
     <t xml:space="preserve">ссимкь биркьий</t>
   </si>
   <si>
-    <t xml:space="preserve">ссимкь бик1вий</t>
+    <t xml:space="preserve">ссимкь бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">СЛЕЗА</t>
@@ -12586,7 +12586,7 @@
     <t xml:space="preserve">FEAR</t>
   </si>
   <si>
-    <t xml:space="preserve">урух бик1вий</t>
+    <t xml:space="preserve">урух бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">урух бирхвий</t>
@@ -12601,7 +12601,7 @@
     <t xml:space="preserve">FRIGHTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">урк1 агъий</t>
+    <t xml:space="preserve">уркӀ агъий</t>
   </si>
   <si>
     <t xml:space="preserve">This refers to a moment, like when a person makes a sound, etc.</t>
@@ -12610,7 +12610,7 @@
     <t xml:space="preserve">check what to do with concept</t>
   </si>
   <si>
-    <t xml:space="preserve">урк1 игъий</t>
+    <t xml:space="preserve">уркӀ игъий</t>
   </si>
   <si>
     <t xml:space="preserve">урух баркьий</t>
@@ -12625,10 +12625,10 @@
     <t xml:space="preserve">CHOOSE</t>
   </si>
   <si>
-    <t xml:space="preserve">дик1ар баркьий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дик1ар биркьий</t>
+    <t xml:space="preserve">дикӀар баркьий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дикӀар биркьий</t>
   </si>
   <si>
     <t xml:space="preserve">ОБМАНЫВАТЬ</t>
@@ -12658,7 +12658,7 @@
     <t xml:space="preserve">GOOD</t>
   </si>
   <si>
-    <t xml:space="preserve">г1ях1(це)</t>
+    <t xml:space="preserve">гӀяхӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ПЛОХОЙ</t>
@@ -12814,7 +12814,7 @@
     <t xml:space="preserve">INSANE</t>
   </si>
   <si>
-    <t xml:space="preserve">бях1(це)</t>
+    <t xml:space="preserve">бяхӀ(це)</t>
   </si>
   <si>
     <t xml:space="preserve">ОБУЧАТЬ</t>
@@ -13057,7 +13057,7 @@
     <t xml:space="preserve">SING</t>
   </si>
   <si>
-    <t xml:space="preserve">далай бик1вий</t>
+    <t xml:space="preserve">далай бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ПЕСНЯ</t>
@@ -13078,7 +13078,7 @@
     <t xml:space="preserve">SHOUT</t>
   </si>
   <si>
-    <t xml:space="preserve">вяв бик1вий</t>
+    <t xml:space="preserve">вяв бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">ШЕПТАТЬ</t>
@@ -13087,7 +13087,7 @@
     <t xml:space="preserve">WHISPER</t>
   </si>
   <si>
-    <t xml:space="preserve">шуршур бик1вий</t>
+    <t xml:space="preserve">шуршур бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">СВИСТЕТЬ</t>
@@ -13096,10 +13096,10 @@
     <t xml:space="preserve">WHISTLE</t>
   </si>
   <si>
-    <t xml:space="preserve">хьвит1 бик1вий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">хьвит1 баркьий</t>
+    <t xml:space="preserve">хьвитӀ бикӀвий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хьвитӀ баркьий</t>
   </si>
   <si>
     <t xml:space="preserve">РАЗГОВАРИВАТЬ</t>
@@ -13108,7 +13108,7 @@
     <t xml:space="preserve">TALK</t>
   </si>
   <si>
-    <t xml:space="preserve">гъай бик1вий</t>
+    <t xml:space="preserve">гъай бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">СКАЗАТЬ</t>
@@ -13240,10 +13240,10 @@
     <t xml:space="preserve">CALL</t>
   </si>
   <si>
-    <t xml:space="preserve">вяв берч1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">вяв бурч1ий</t>
+    <t xml:space="preserve">вяв берчӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">вяв бурчӀий</t>
   </si>
   <si>
     <t xml:space="preserve">вяв гьаъий</t>
@@ -13258,10 +13258,10 @@
     <t xml:space="preserve">WRITE</t>
   </si>
   <si>
-    <t xml:space="preserve">белк1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">лук1ий</t>
+    <t xml:space="preserve">белкӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">лукӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ЧИТАТЬ</t>
@@ -13270,10 +13270,10 @@
     <t xml:space="preserve">READ</t>
   </si>
   <si>
-    <t xml:space="preserve">белч1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">буч1ий</t>
+    <t xml:space="preserve">белчӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бучӀий</t>
   </si>
   <si>
     <t xml:space="preserve">БУМАГА</t>
@@ -13420,10 +13420,10 @@
     <t xml:space="preserve">GUEST</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яхху1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">г1яхвле</t>
+    <t xml:space="preserve">гӀяххуӀл</t>
+  </si>
+  <si>
+    <t xml:space="preserve">гӀяхвле</t>
   </si>
   <si>
     <t xml:space="preserve">ПОМОГАТЬ</t>
@@ -13444,13 +13444,13 @@
     <t xml:space="preserve">FIGHT (VB)</t>
   </si>
   <si>
-    <t xml:space="preserve">бирх1ий</t>
+    <t xml:space="preserve">бирхӀий</t>
   </si>
   <si>
     <t xml:space="preserve">birħij</t>
   </si>
   <si>
-    <t xml:space="preserve">бих1ий</t>
+    <t xml:space="preserve">бихӀий</t>
   </si>
   <si>
     <t xml:space="preserve">biħij</t>
@@ -13462,10 +13462,10 @@
     <t xml:space="preserve">WAR</t>
   </si>
   <si>
-    <t xml:space="preserve">дяг1ви</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дяг1вте</t>
+    <t xml:space="preserve">дягӀви</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дягӀвте</t>
   </si>
   <si>
     <t xml:space="preserve">ВООРУЖЕННЫЙ ОТРЯД</t>
@@ -13534,10 +13534,10 @@
     <t xml:space="preserve">SCABBARD</t>
   </si>
   <si>
-    <t xml:space="preserve">кьу1рт1ала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">кьу1рт1алме</t>
+    <t xml:space="preserve">кьуӀртӀала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кьуӀртӀалме</t>
   </si>
   <si>
     <t xml:space="preserve">РУКОЯТКА</t>
@@ -13585,10 +13585,10 @@
     <t xml:space="preserve">TOWER</t>
   </si>
   <si>
-    <t xml:space="preserve">ккалг1я</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ккалг1не</t>
+    <t xml:space="preserve">ккалгӀя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ккалгӀне</t>
   </si>
   <si>
     <t xml:space="preserve">РЫБАЦКАЯ СЕТЬ</t>
@@ -13603,7 +13603,7 @@
     <t xml:space="preserve">HUNT</t>
   </si>
   <si>
-    <t xml:space="preserve">г1яярре баший</t>
+    <t xml:space="preserve">гӀяярре баший</t>
   </si>
   <si>
     <t xml:space="preserve">ʡaˁaˁrre wašij</t>
@@ -13684,10 +13684,10 @@
     <t xml:space="preserve">STEAL</t>
   </si>
   <si>
-    <t xml:space="preserve">биг1ий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">билг1ий</t>
+    <t xml:space="preserve">бигӀий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">билгӀий</t>
   </si>
   <si>
     <t xml:space="preserve">ВОР</t>
@@ -13696,10 +13696,10 @@
     <t xml:space="preserve">THIEF</t>
   </si>
   <si>
-    <t xml:space="preserve">билг1у1т1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">билг1у1т1е</t>
+    <t xml:space="preserve">билгӀуӀтӀ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">билгӀуӀтӀе</t>
   </si>
   <si>
     <t xml:space="preserve">МОЛИТЬСЯ</t>
@@ -13777,7 +13777,7 @@
     <t xml:space="preserve">RING (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">зангъ бик1вий</t>
+    <t xml:space="preserve">зангъ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">СКРИПЕТЬ</t>
@@ -13786,7 +13786,7 @@
     <t xml:space="preserve">SQUEAK</t>
   </si>
   <si>
-    <t xml:space="preserve">гъярч1 бик1вий</t>
+    <t xml:space="preserve">гъярчӀ бикӀвий</t>
   </si>
   <si>
     <t xml:space="preserve">БЫТЬ ДОЛЖНЫМ, ОБЯЗАННЫМ</t>
@@ -14475,7 +14475,6 @@
         <charset val="1"/>
         <family val="2"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -14553,12 +14552,12 @@
   <dimension ref="A1:AMJ2142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="K2109" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="K2097" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2139" activeCellId="0" sqref="A2139"/>
+      <selection pane="bottomLeft" activeCell="L2111" activeCellId="0" sqref="L2111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="5.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.15"/>
@@ -14574,7 +14573,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="17.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="15" style="4" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -71400,7 +71398,7 @@
       <c r="K2142" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AD2139"/>
+  <autoFilter ref="B1:K2139"/>
   <conditionalFormatting sqref="D1:IO1">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(D1))&gt;0</formula>

</xml_diff>